<commit_message>
mean Anomaly jupiter moon
</commit_message>
<xml_diff>
--- a/src/app/scene/data/jupiter.xlsx
+++ b/src/app/scene/data/jupiter.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="862" uniqueCount="736">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="878" uniqueCount="752">
   <si>
     <t>Metis</t>
   </si>
@@ -2254,6 +2254,54 @@
   </si>
   <si>
     <t>718.37</t>
+  </si>
+  <si>
+    <t>356.6</t>
+  </si>
+  <si>
+    <t>282.4</t>
+  </si>
+  <si>
+    <t>169.9</t>
+  </si>
+  <si>
+    <t>201.41718</t>
+  </si>
+  <si>
+    <t>168.7</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 236.9</t>
+  </si>
+  <si>
+    <t>91.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 25.53</t>
+  </si>
+  <si>
+    <t>259.5</t>
+  </si>
+  <si>
+    <t>344.4</t>
+  </si>
+  <si>
+    <t>236.9</t>
+  </si>
+  <si>
+    <t>161.6</t>
+  </si>
+  <si>
+    <t>70.8</t>
+  </si>
+  <si>
+    <t>77.5</t>
+  </si>
+  <si>
+    <t>161.3</t>
+  </si>
+  <si>
+    <t>284.4</t>
   </si>
 </sst>
 </file>
@@ -2331,7 +2379,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2383,6 +2431,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFEEEEEE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2441,7 +2495,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2573,18 +2627,6 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2606,6 +2648,19 @@
     <xf numFmtId="0" fontId="9" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -2889,8 +2944,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P153"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="I68" sqref="I68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2905,10 +2960,10 @@
       <c r="A1" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="54" t="s">
         <v>91</v>
       </c>
-      <c r="C1" s="45" t="s">
+      <c r="C1" s="52" t="s">
         <v>92</v>
       </c>
       <c r="D1" s="23" t="s">
@@ -2925,8 +2980,8 @@
       <c r="A2" s="22" t="s">
         <v>90</v>
       </c>
-      <c r="B2" s="48"/>
-      <c r="C2" s="46"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="53"/>
       <c r="D2" s="22" t="s">
         <v>94</v>
       </c>
@@ -2983,7 +3038,7 @@
         <v>METIS</v>
       </c>
       <c r="I3" t="str">
-        <f>LOWER(SUBSTITUTE(SUBSTITUTE(B3," ","-"),"/","/"))</f>
+        <f>LOWER(SUBSTITUTE(SUBSTITUTE(B3," ","-"),"/","_"))</f>
         <v>metis</v>
       </c>
       <c r="J3" s="28" t="str">
@@ -3007,7 +3062,7 @@
   semiMajorAxis: "&amp;E3&amp;",
   eccentricity: "&amp;F3&amp;",
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: "&amp;G3&amp;",
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -3024,7 +3079,7 @@
   semiMajorAxis: 128852,
   eccentricity: 0.0077,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 276.047,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -3059,7 +3114,7 @@
         <v>ADRASTEA</v>
       </c>
       <c r="I4" t="str">
-        <f t="shared" ref="I4:I67" si="2">LOWER(SUBSTITUTE(SUBSTITUTE(B4," ","-"),"/","/"))</f>
+        <f t="shared" ref="I4:I67" si="2">LOWER(SUBSTITUTE(SUBSTITUTE(B4," ","-"),"/","_"))</f>
         <v>adrastea</v>
       </c>
       <c r="J4" s="28" t="str">
@@ -3083,7 +3138,7 @@
   semiMajorAxis: "&amp;E4&amp;",
   eccentricity: "&amp;F4&amp;",
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: "&amp;G4&amp;",
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -3100,7 +3155,7 @@
   semiMajorAxis: 129000,
   eccentricity: 0.0063,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 135.673,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -3160,7 +3215,7 @@
   semiMajorAxis: 181366,
   eccentricity: 0.0075,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 185.194,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -3220,7 +3275,7 @@
   semiMajorAxis: 222452,
   eccentricity: 0.0180,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 135.956,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -3280,7 +3335,7 @@
   semiMajorAxis: 421700,
   eccentricity: 0.0041,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 342.021,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -3340,7 +3395,7 @@
   semiMajorAxis: 671034,
   eccentricity: 0.0094,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 171.016,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -3400,7 +3455,7 @@
   semiMajorAxis: 1070412,
   eccentricity: 0.0011,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 317.540,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -3460,7 +3515,7 @@
   semiMajorAxis: 1882709,
   eccentricity: 0.0074,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 181.408,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -3520,7 +3575,7 @@
   semiMajorAxis: 7405000,
   eccentricity: 0.2514,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 313.051,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -3580,7 +3635,7 @@
   semiMajorAxis: 11196000,
   eccentricity: 0.1648,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 230.352,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -3606,9 +3661,8 @@
       <c r="F13" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="G13" t="str">
-        <f t="shared" si="0"/>
-        <v>null</v>
+      <c r="G13" s="56" t="s">
+        <v>736</v>
       </c>
       <c r="H13" t="str">
         <f t="shared" si="1"/>
@@ -3640,7 +3694,7 @@
   semiMajorAxis: 11348700,
   eccentricity: 0.1043,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 356.6,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -3666,9 +3720,8 @@
       <c r="F14" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="G14" t="str">
-        <f t="shared" si="0"/>
-        <v>null</v>
+      <c r="G14" s="56" t="s">
+        <v>737</v>
       </c>
       <c r="H14" t="str">
         <f t="shared" si="1"/>
@@ -3700,7 +3753,7 @@
   semiMajorAxis: 11462300,
   eccentricity: 0.2084,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 282.4,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -3760,7 +3813,7 @@
   semiMajorAxis: 11497400,
   eccentricity: 0.1510,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 66.874,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -3820,7 +3873,7 @@
   semiMajorAxis: 11628300,
   eccentricity: 0.1377,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 330.475,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -3880,7 +3933,7 @@
   semiMajorAxis: 11671600,
   eccentricity: 0.2079,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 330.985,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -3906,9 +3959,8 @@
       <c r="F18" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="G18" t="str">
-        <f t="shared" si="0"/>
-        <v>null</v>
+      <c r="G18" s="56" t="s">
+        <v>738</v>
       </c>
       <c r="H18" t="str">
         <f t="shared" si="1"/>
@@ -3940,7 +3992,7 @@
   semiMajorAxis: 12304900,
   eccentricity: 0.2606,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 169.9,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -4000,7 +4052,7 @@
   semiMajorAxis: 17151800,
   eccentricity: 0.4967,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 337.062,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -4026,9 +4078,8 @@
       <c r="F20" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="G20" t="str">
-        <f t="shared" si="0"/>
-        <v>null</v>
+      <c r="G20" s="56" t="s">
+        <v>739</v>
       </c>
       <c r="H20" t="str">
         <f t="shared" si="1"/>
@@ -4060,7 +4111,7 @@
   semiMajorAxis: 18819000,
   eccentricity: 0.2018,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 201.41718,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -4120,7 +4171,7 @@
   semiMajorAxis: 19593900,
   eccentricity: 0.1402,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 70.243,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -4146,9 +4197,8 @@
       <c r="F22" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="G22" t="str">
-        <f t="shared" si="0"/>
-        <v>null</v>
+      <c r="G22" s="56" t="s">
+        <v>740</v>
       </c>
       <c r="H22" t="str">
         <f t="shared" si="1"/>
@@ -4180,7 +4230,7 @@
   semiMajorAxis: 20126300,
   eccentricity: 0.4104,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 168.7,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -4216,7 +4266,7 @@
       </c>
       <c r="I23" t="str">
         <f t="shared" si="2"/>
-        <v>s/2003-j-18</v>
+        <v>s_2003-j-18</v>
       </c>
       <c r="J23" s="28" t="str">
         <f t="shared" si="3"/>
@@ -4229,7 +4279,7 @@
       <c r="L23" t="str">
         <f t="shared" si="5"/>
         <v>export const S_2003_J_18: CelestialBody = {
-  id: 's/2003-j-18',
+  id: 's_2003-j-18',
   position: {
     x: 0,
     y: 0
@@ -4240,7 +4290,7 @@
   semiMajorAxis: 20348800,
   eccentricity: 0.0465,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 202.160,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -4276,7 +4326,7 @@
       </c>
       <c r="I24" t="str">
         <f t="shared" si="2"/>
-        <v>s/2010-j-2</v>
+        <v>s_2010-j-2</v>
       </c>
       <c r="J24" s="28" t="str">
         <f t="shared" si="3"/>
@@ -4289,7 +4339,7 @@
       <c r="L24" t="str">
         <f t="shared" si="5"/>
         <v>export const S_2010_J_2: CelestialBody = {
-  id: 's/2010-j-2',
+  id: 's_2010-j-2',
   position: {
     x: 0,
     y: 0
@@ -4300,7 +4350,7 @@
   semiMajorAxis: 20436700,
   eccentricity: 0.3403,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 312.074,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -4360,7 +4410,7 @@
   semiMajorAxis: 20479500,
   eccentricity: 0.1331,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 43.659,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -4396,7 +4446,7 @@
       </c>
       <c r="I26" t="str">
         <f t="shared" si="2"/>
-        <v>s/2003-j-16</v>
+        <v>s_2003-j-16</v>
       </c>
       <c r="J26" s="28" t="str">
         <f t="shared" si="3"/>
@@ -4409,7 +4459,7 @@
       <c r="L26" t="str">
         <f t="shared" si="5"/>
         <v>export const S_2003_J_16: CelestialBody = {
-  id: 's/2003-j-16',
+  id: 's_2003-j-16',
   position: {
     x: 0,
     y: 0
@@ -4420,7 +4470,7 @@
   semiMajorAxis: 20512500,
   eccentricity: 0.3331,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 307.563,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -4456,7 +4506,7 @@
       </c>
       <c r="I27" t="str">
         <f t="shared" si="2"/>
-        <v>s/2003-j-2</v>
+        <v>s_2003-j-2</v>
       </c>
       <c r="J27" s="28" t="str">
         <f t="shared" si="3"/>
@@ -4469,7 +4519,7 @@
       <c r="L27" t="str">
         <f t="shared" si="5"/>
         <v>export const S_2003_J_2: CelestialBody = {
-  id: 's/2003-j-2',
+  id: 's_2003-j-2',
   position: {
     x: 0,
     y: 0
@@ -4480,7 +4530,7 @@
   semiMajorAxis: 20554400,
   eccentricity: 0.2777,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 237.932,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -4540,7 +4590,7 @@
   semiMajorAxis: 20583300,
   eccentricity: 0.1096,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 333.101,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -4566,9 +4616,8 @@
       <c r="F29" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="G29" t="str">
-        <f t="shared" si="0"/>
-        <v>null</v>
+      <c r="G29" s="56" t="s">
+        <v>741</v>
       </c>
       <c r="H29" t="str">
         <f t="shared" si="1"/>
@@ -4576,7 +4625,7 @@
       </c>
       <c r="I29" t="str">
         <f t="shared" si="2"/>
-        <v>s/2017-j-7</v>
+        <v>s_2017-j-7</v>
       </c>
       <c r="J29" s="28" t="str">
         <f t="shared" si="3"/>
@@ -4589,7 +4638,7 @@
       <c r="L29" t="str">
         <f t="shared" si="5"/>
         <v>export const S_2017_J_7: CelestialBody = {
-  id: 's/2017-j-7',
+  id: 's_2017-j-7',
   position: {
     x: 0,
     y: 0
@@ -4600,7 +4649,7 @@
   semiMajorAxis: 20600100,
   eccentricity: 0.2626,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly:  236.9,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -4660,7 +4709,7 @@
   semiMajorAxis: 20666200,
   eccentricity: 0.1981,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 131.854,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -4720,7 +4769,7 @@
   semiMajorAxis: 20682900,
   eccentricity: 0.2959,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 117.480,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -4780,7 +4829,7 @@
   semiMajorAxis: 20712800,
   eccentricity: 0.1770,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 238.786,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -4840,7 +4889,7 @@
   semiMajorAxis: 20893300,
   eccentricity: 0.1709,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 268.013,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -4866,9 +4915,8 @@
       <c r="F34" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="G34" t="str">
-        <f t="shared" si="0"/>
-        <v>null</v>
+      <c r="G34" s="56" t="s">
+        <v>742</v>
       </c>
       <c r="H34" t="str">
         <f t="shared" si="1"/>
@@ -4876,7 +4924,7 @@
       </c>
       <c r="I34" t="str">
         <f t="shared" si="2"/>
-        <v>s/2017-j-3</v>
+        <v>s_2017-j-3</v>
       </c>
       <c r="J34" s="28" t="str">
         <f t="shared" si="3"/>
@@ -4889,7 +4937,7 @@
       <c r="L34" t="str">
         <f t="shared" si="5"/>
         <v>export const S_2017_J_3: CelestialBody = {
-  id: 's/2017-j-3',
+  id: 's_2017-j-3',
   position: {
     x: 0,
     y: 0
@@ -4900,7 +4948,7 @@
   semiMajorAxis: 20976900,
   eccentricity: 0.1907,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 91.2,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -4960,7 +5008,7 @@
   semiMajorAxis: 21042500,
   eccentricity: 0.1747,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 253.384,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -5020,7 +5068,7 @@
   semiMajorAxis: 21064100,
   eccentricity: 0.3428,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 256.860,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -5046,9 +5094,8 @@
       <c r="F37" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="G37" t="str">
-        <f t="shared" si="0"/>
-        <v>null</v>
+      <c r="G37" s="56" t="s">
+        <v>743</v>
       </c>
       <c r="H37" t="str">
         <f t="shared" si="1"/>
@@ -5056,7 +5103,7 @@
       </c>
       <c r="I37" t="str">
         <f t="shared" si="2"/>
-        <v>s/2016-j-1</v>
+        <v>s_2016-j-1</v>
       </c>
       <c r="J37" s="28" t="str">
         <f t="shared" si="3"/>
@@ -5069,7 +5116,7 @@
       <c r="L37" t="str">
         <f t="shared" si="5"/>
         <v>export const S_2016_J_1: CelestialBody = {
-  id: 's/2016-j-1',
+  id: 's_2016-j-1',
   position: {
     x: 0,
     y: 0
@@ -5080,7 +5127,7 @@
   semiMajorAxis: 21154000,
   eccentricity: 0.1294,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly:  25.53,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -5140,7 +5187,7 @@
   semiMajorAxis: 21171000,
   eccentricity: 0.4838,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 204.517,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -5200,7 +5247,7 @@
   semiMajorAxis: 21280200,
   eccentricity: 0.1602,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 215.956,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -5260,7 +5307,7 @@
   semiMajorAxis: 21431800,
   eccentricity: 0.3295,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 213.675,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -5286,9 +5333,8 @@
       <c r="F41" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="G41" t="str">
-        <f t="shared" si="0"/>
-        <v>null</v>
+      <c r="G41" s="56" t="s">
+        <v>744</v>
       </c>
       <c r="H41" t="str">
         <f t="shared" si="1"/>
@@ -5296,7 +5342,7 @@
       </c>
       <c r="I41" t="str">
         <f t="shared" si="2"/>
-        <v>s/2017-j-9</v>
+        <v>s_2017-j-9</v>
       </c>
       <c r="J41" s="28" t="str">
         <f t="shared" si="3"/>
@@ -5309,7 +5355,7 @@
       <c r="L41" t="str">
         <f t="shared" si="5"/>
         <v>export const S_2017_J_9: CelestialBody = {
-  id: 's/2017-j-9',
+  id: 's_2017-j-9',
   position: {
     x: 0,
     y: 0
@@ -5320,7 +5366,7 @@
   semiMajorAxis: 21492900,
   eccentricity: 0.2524,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 259.5,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -5356,7 +5402,7 @@
       </c>
       <c r="I42" t="str">
         <f t="shared" si="2"/>
-        <v>s/2003-j-12</v>
+        <v>s_2003-j-12</v>
       </c>
       <c r="J42" s="28" t="str">
         <f t="shared" si="3"/>
@@ -5369,7 +5415,7 @@
       <c r="L42" t="str">
         <f t="shared" si="5"/>
         <v>export const S_2003_J_12: CelestialBody = {
-  id: 's/2003-j-12',
+  id: 's_2003-j-12',
   position: {
     x: 0,
     y: 0
@@ -5380,7 +5426,7 @@
   semiMajorAxis: 21557700,
   eccentricity: 0.3657,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 38.543,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -5416,7 +5462,7 @@
       </c>
       <c r="I43" t="str">
         <f t="shared" si="2"/>
-        <v>s/2003-j-4</v>
+        <v>s_2003-j-4</v>
       </c>
       <c r="J43" s="28" t="str">
         <f t="shared" si="3"/>
@@ -5429,7 +5475,7 @@
       <c r="L43" t="str">
         <f t="shared" si="5"/>
         <v>export const S_2003_J_4: CelestialBody = {
-  id: 's/2003-j-4',
+  id: 's_2003-j-4',
   position: {
     x: 0,
     y: 0
@@ -5440,7 +5486,7 @@
   semiMajorAxis: 22048600,
   eccentricity: 0.4967,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 260.480,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -5500,7 +5546,7 @@
   semiMajorAxis: 22354300,
   eccentricity: 0.2052,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 267.136,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -5560,7 +5606,7 @@
   semiMajorAxis: 22386500,
   eccentricity: 0.3150,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 105.000,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -5620,7 +5666,7 @@
   semiMajorAxis: 22408800,
   eccentricity: 0.1854,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 141.667,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -5680,7 +5726,7 @@
   semiMajorAxis: 22433500,
   eccentricity: 0.3257,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 94.756,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -5706,9 +5752,8 @@
       <c r="F48" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="G48" t="str">
-        <f t="shared" si="0"/>
-        <v>null</v>
+      <c r="G48" s="56" t="s">
+        <v>745</v>
       </c>
       <c r="H48" t="str">
         <f t="shared" si="1"/>
@@ -5716,7 +5761,7 @@
       </c>
       <c r="I48" t="str">
         <f t="shared" si="2"/>
-        <v>s/2017-j-2</v>
+        <v>s_2017-j-2</v>
       </c>
       <c r="J48" s="28" t="str">
         <f t="shared" si="3"/>
@@ -5729,7 +5774,7 @@
       <c r="L48" t="str">
         <f t="shared" si="5"/>
         <v>export const S_2017_J_2: CelestialBody = {
-  id: 's/2017-j-2',
+  id: 's_2017-j-2',
   position: {
     x: 0,
     y: 0
@@ -5740,7 +5785,7 @@
   semiMajorAxis: 22472900,
   eccentricity: 0.3852,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 344.4,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -5766,9 +5811,8 @@
       <c r="F49" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="G49" t="str">
-        <f t="shared" si="0"/>
-        <v>null</v>
+      <c r="G49" s="56" t="s">
+        <v>746</v>
       </c>
       <c r="H49" t="str">
         <f t="shared" si="1"/>
@@ -5776,7 +5820,7 @@
       </c>
       <c r="I49" t="str">
         <f t="shared" si="2"/>
-        <v>s/2017-j-6</v>
+        <v>s_2017-j-6</v>
       </c>
       <c r="J49" s="28" t="str">
         <f t="shared" si="3"/>
@@ -5789,7 +5833,7 @@
       <c r="L49" t="str">
         <f t="shared" si="5"/>
         <v>export const S_2017_J_6: CelestialBody = {
-  id: 's/2017-j-6',
+  id: 's_2017-j-6',
   position: {
     x: 0,
     y: 0
@@ -5800,7 +5844,7 @@
   semiMajorAxis: 22543800,
   eccentricity: 0.3226,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 236.9,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -5860,7 +5904,7 @@
   semiMajorAxis: 22576700,
   eccentricity: 0.2790,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 204.846,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -5920,7 +5964,7 @@
   semiMajorAxis: 22579900,
   eccentricity: 0.2295,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 233.375,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -5956,7 +6000,7 @@
       </c>
       <c r="I52" t="str">
         <f t="shared" si="2"/>
-        <v>s/2003-j-19</v>
+        <v>s_2003-j-19</v>
       </c>
       <c r="J52" s="28" t="str">
         <f t="shared" si="3"/>
@@ -5969,7 +6013,7 @@
       <c r="L52" t="str">
         <f t="shared" si="5"/>
         <v>export const S_2003_J_19: CelestialBody = {
-  id: 's/2003-j-19',
+  id: 's_2003-j-19',
   position: {
     x: 0,
     y: 0
@@ -5980,7 +6024,7 @@
   semiMajorAxis: 22752500,
   eccentricity: 0.2928,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 223.035,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -6040,7 +6084,7 @@
   semiMajorAxis: 22776700,
   eccentricity: 0.2159,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 124.941,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -6076,7 +6120,7 @@
       </c>
       <c r="I54" t="str">
         <f t="shared" si="2"/>
-        <v>s/2003-j-10</v>
+        <v>s_2003-j-10</v>
       </c>
       <c r="J54" s="28" t="str">
         <f t="shared" si="3"/>
@@ -6089,7 +6133,7 @@
       <c r="L54" t="str">
         <f t="shared" si="5"/>
         <v>export const S_2003_J_10: CelestialBody = {
-  id: 's/2003-j-10',
+  id: 's_2003-j-10',
   position: {
     x: 0,
     y: 0
@@ -6100,7 +6144,7 @@
   semiMajorAxis: 22896200,
   eccentricity: 0.2066,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 258.937,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -6160,7 +6204,7 @@
   semiMajorAxis: 22933400,
   eccentricity: 0.4290,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 142.035,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -6186,9 +6230,8 @@
       <c r="F56" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="G56" t="str">
-        <f t="shared" si="0"/>
-        <v>null</v>
+      <c r="G56" s="56" t="s">
+        <v>747</v>
       </c>
       <c r="H56" t="str">
         <f t="shared" si="1"/>
@@ -6220,7 +6263,7 @@
   semiMajorAxis: 22939900,
   eccentricity: 0.3013,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 161.6,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -6280,7 +6323,7 @@
   semiMajorAxis: 22965200,
   eccentricity: 0.6079,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 128.345,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -6340,7 +6383,7 @@
   semiMajorAxis: 22967800,
   eccentricity: 0.2097,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 215.443,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -6376,7 +6419,7 @@
       </c>
       <c r="I59" t="str">
         <f t="shared" si="2"/>
-        <v>s/2010-j-1</v>
+        <v>s_2010-j-1</v>
       </c>
       <c r="J59" s="28" t="str">
         <f t="shared" si="3"/>
@@ -6389,7 +6432,7 @@
       <c r="L59" t="str">
         <f t="shared" si="5"/>
         <v>export const S_2010_J_1: CelestialBody = {
-  id: 's/2010-j-1',
+  id: 's_2010-j-1',
   position: {
     x: 0,
     y: 0
@@ -6400,7 +6443,7 @@
   semiMajorAxis: 22986900,
   eccentricity: 0.2937,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 160.525,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -6460,7 +6503,7 @@
   semiMajorAxis: 23119300,
   eccentricity: 0.4362,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 279.769,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -6520,7 +6563,7 @@
   semiMajorAxis: 23146500,
   eccentricity: 0.3455,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 174.044,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -6546,9 +6589,8 @@
       <c r="F62" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="G62" t="str">
-        <f t="shared" si="0"/>
-        <v>null</v>
+      <c r="G62" s="56" t="s">
+        <v>748</v>
       </c>
       <c r="H62" t="str">
         <f t="shared" si="1"/>
@@ -6556,7 +6598,7 @@
       </c>
       <c r="I62" t="str">
         <f t="shared" si="2"/>
-        <v>s/2017-j-8</v>
+        <v>s_2017-j-8</v>
       </c>
       <c r="J62" s="28" t="str">
         <f t="shared" si="3"/>
@@ -6569,7 +6611,7 @@
       <c r="L62" t="str">
         <f t="shared" si="5"/>
         <v>export const S_2017_J_8: CelestialBody = {
-  id: 's/2017-j-8',
+  id: 's_2017-j-8',
   position: {
     x: 0,
     y: 0
@@ -6580,7 +6622,7 @@
   semiMajorAxis: 23173700,
   eccentricity: 0.2039,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 70.8,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -6640,7 +6682,7 @@
   semiMajorAxis: 23214500,
   eccentricity: 0.2975,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 287.689,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -6666,9 +6708,8 @@
       <c r="F64" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="G64" t="str">
-        <f t="shared" si="0"/>
-        <v>null</v>
+      <c r="G64" s="56" t="s">
+        <v>749</v>
       </c>
       <c r="H64" t="str">
         <f t="shared" si="1"/>
@@ -6676,7 +6717,7 @@
       </c>
       <c r="I64" t="str">
         <f t="shared" si="2"/>
-        <v>s/2017-j-5</v>
+        <v>s_2017-j-5</v>
       </c>
       <c r="J64" s="28" t="str">
         <f t="shared" si="3"/>
@@ -6689,7 +6730,7 @@
       <c r="L64" t="str">
         <f t="shared" si="5"/>
         <v>export const S_2017_J_5: CelestialBody = {
-  id: 's/2017-j-5',
+  id: 's_2017-j-5',
   position: {
     x: 0,
     y: 0
@@ -6700,7 +6741,7 @@
   semiMajorAxis: 23352500,
   eccentricity: 0.2460,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 77.5,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -6760,7 +6801,7 @@
   semiMajorAxis: 23377400,
   eccentricity: 0.2660,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 255.702,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -6820,7 +6861,7 @@
   semiMajorAxis: 23422300,
   eccentricity: 0.3358,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 236.950,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -6880,7 +6921,7 @@
   semiMajorAxis: 23512200,
   eccentricity: 0.2893,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 212.853,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -6915,7 +6956,7 @@
         <v>KALLICHORE</v>
       </c>
       <c r="I68" t="str">
-        <f t="shared" ref="I68:I81" si="8">LOWER(SUBSTITUTE(SUBSTITUTE(B68," ","-"),"/","/"))</f>
+        <f t="shared" ref="I68:I81" si="8">LOWER(SUBSTITUTE(SUBSTITUTE(B68," ","-"),"/","_"))</f>
         <v>kallichore</v>
       </c>
       <c r="J68" s="28" t="str">
@@ -6939,7 +6980,7 @@
   semiMajorAxis: "&amp;E68&amp;",
   eccentricity: "&amp;F68&amp;",
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: "&amp;G68&amp;",
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -6956,7 +6997,7 @@
   semiMajorAxis: 23552900,
   eccentricity: 0.3183,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 55.937,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -6992,7 +7033,7 @@
       </c>
       <c r="I69" t="str">
         <f t="shared" si="8"/>
-        <v>s/2011-j-1</v>
+        <v>s_2011-j-1</v>
       </c>
       <c r="J69" s="28" t="str">
         <f t="shared" si="9"/>
@@ -7005,7 +7046,7 @@
       <c r="L69" t="str">
         <f t="shared" si="11"/>
         <v>export const S_2011_J_1: CelestialBody = {
-  id: 's/2011-j-1',
+  id: 's_2011-j-1',
   position: {
     x: 0,
     y: 0
@@ -7016,7 +7057,7 @@
   semiMajorAxis: 23714400,
   eccentricity: 0.3193,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 256.027,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -7042,9 +7083,8 @@
       <c r="F70" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="G70" t="str">
-        <f t="shared" si="6"/>
-        <v>null</v>
+      <c r="G70" s="56" t="s">
+        <v>750</v>
       </c>
       <c r="H70" t="str">
         <f t="shared" si="7"/>
@@ -7052,7 +7092,7 @@
       </c>
       <c r="I70" t="str">
         <f t="shared" si="8"/>
-        <v>s/2017-j-1</v>
+        <v>s_2017-j-1</v>
       </c>
       <c r="J70" s="28" t="str">
         <f t="shared" si="9"/>
@@ -7065,7 +7105,7 @@
       <c r="L70" t="str">
         <f t="shared" si="11"/>
         <v>export const S_2017_J_1: CelestialBody = {
-  id: 's/2017-j-1',
+  id: 's_2017-j-1',
   position: {
     x: 0,
     y: 0
@@ -7076,7 +7116,7 @@
   semiMajorAxis: 23753600,
   eccentricity: 0.4500,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 161.3,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -7136,7 +7176,7 @@
   semiMajorAxis: 23848300,
   eccentricity: 0.2705,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 267.454,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -7196,7 +7236,7 @@
   semiMajorAxis: 23926500,
   eccentricity: 0.2367,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 39.713,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -7222,9 +7262,8 @@
       <c r="F73" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="G73" t="str">
-        <f t="shared" si="6"/>
-        <v>null</v>
+      <c r="G73" s="56" t="s">
+        <v>751</v>
       </c>
       <c r="H73" t="str">
         <f t="shared" si="7"/>
@@ -7256,7 +7295,7 @@
   semiMajorAxis: 23934500,
   eccentricity: 0.2413,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 284.4,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -7316,7 +7355,7 @@
   semiMajorAxis: 23999700,
   eccentricity: 0.2347,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 33.416,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -7352,7 +7391,7 @@
       </c>
       <c r="I75" t="str">
         <f t="shared" si="8"/>
-        <v>s/2011-j-2</v>
+        <v>s_2011-j-2</v>
       </c>
       <c r="J75" s="28" t="str">
         <f t="shared" si="9"/>
@@ -7365,7 +7404,7 @@
       <c r="L75" t="str">
         <f t="shared" si="11"/>
         <v>export const S_2011_J_2: CelestialBody = {
-  id: 's/2011-j-2',
+  id: 's_2011-j-2',
   position: {
     x: 0,
     y: 0
@@ -7376,7 +7415,7 @@
   semiMajorAxis: 24114700,
   eccentricity: 0.1729,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 285.597,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -7412,7 +7451,7 @@
       </c>
       <c r="I76" t="str">
         <f t="shared" si="8"/>
-        <v>s/2003-j-9</v>
+        <v>s_2003-j-9</v>
       </c>
       <c r="J76" s="28" t="str">
         <f t="shared" si="9"/>
@@ -7425,7 +7464,7 @@
       <c r="L76" t="str">
         <f t="shared" si="11"/>
         <v>export const S_2003_J_9: CelestialBody = {
-  id: 's/2003-j-9',
+  id: 's_2003-j-9',
   position: {
     x: 0,
     y: 0
@@ -7436,7 +7475,7 @@
   semiMajorAxis: 24168700,
   eccentricity: 0.1702,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 348.415,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -7496,7 +7535,7 @@
   semiMajorAxis: 24212300,
   eccentricity: 0.3139,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 135.272,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -7556,7 +7595,7 @@
   semiMajorAxis: 24283000,
   eccentricity: 0.3131,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 197.676,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -7592,7 +7631,7 @@
       </c>
       <c r="I79" t="str">
         <f t="shared" si="8"/>
-        <v>s/2003-j-23</v>
+        <v>s_2003-j-23</v>
       </c>
       <c r="J79" s="28" t="str">
         <f t="shared" si="9"/>
@@ -7605,7 +7644,7 @@
       <c r="L79" t="str">
         <f t="shared" si="11"/>
         <v>export const S_2003_J_23: CelestialBody = {
-  id: 's/2003-j-23',
+  id: 's_2003-j-23',
   position: {
     x: 0,
     y: 0
@@ -7616,7 +7655,7 @@
   semiMajorAxis: 24678200,
   eccentricity: 0.3208,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 144.222,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -7676,7 +7715,7 @@
   semiMajorAxis: 24692400,
   eccentricity: 0.3562,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 107.962,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -7736,7 +7775,7 @@
   semiMajorAxis: 24864100,
   eccentricity: 0.1669,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 165.352,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -7744,2232 +7783,2232 @@
       </c>
     </row>
     <row r="85" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B85" s="52" t="s">
+      <c r="B85" s="48" t="s">
         <v>249</v>
       </c>
-      <c r="C85" s="53" t="s">
+      <c r="C85" s="49" t="s">
         <v>250</v>
       </c>
-      <c r="D85" s="53" t="s">
+      <c r="D85" s="49" t="s">
         <v>251</v>
       </c>
-      <c r="E85" s="53" t="s">
+      <c r="E85" s="49" t="s">
         <v>252</v>
       </c>
-      <c r="F85" s="53" t="s">
+      <c r="F85" s="49" t="s">
         <v>253</v>
       </c>
-      <c r="G85" s="53" t="s">
+      <c r="G85" s="49" t="s">
         <v>254</v>
       </c>
-      <c r="H85" s="53" t="s">
+      <c r="H85" s="49" t="s">
         <v>255</v>
       </c>
-      <c r="I85" s="53" t="s">
+      <c r="I85" s="49" t="s">
         <v>256</v>
       </c>
-      <c r="J85" s="53" t="s">
+      <c r="J85" s="49" t="s">
         <v>257</v>
       </c>
-      <c r="K85" s="53"/>
-      <c r="L85" s="53"/>
-      <c r="M85" s="54"/>
+      <c r="K85" s="49"/>
+      <c r="L85" s="49"/>
+      <c r="M85" s="50"/>
     </row>
     <row r="86" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B86" s="52"/>
-      <c r="C86" s="55" t="s">
+      <c r="B86" s="48"/>
+      <c r="C86" s="51" t="s">
         <v>258</v>
       </c>
-      <c r="D86" s="55"/>
-      <c r="E86" s="55" t="s">
+      <c r="D86" s="51"/>
+      <c r="E86" s="51" t="s">
         <v>259</v>
       </c>
-      <c r="F86" s="55" t="s">
+      <c r="F86" s="51" t="s">
         <v>259</v>
       </c>
-      <c r="G86" s="55" t="s">
+      <c r="G86" s="51" t="s">
         <v>259</v>
       </c>
-      <c r="H86" s="55" t="s">
+      <c r="H86" s="51" t="s">
         <v>259</v>
       </c>
-      <c r="I86" s="55" t="s">
+      <c r="I86" s="51" t="s">
         <v>260</v>
       </c>
-      <c r="J86" s="55" t="s">
+      <c r="J86" s="51" t="s">
         <v>261</v>
       </c>
-      <c r="K86" s="55"/>
-      <c r="L86" s="55"/>
-      <c r="M86" s="54"/>
+      <c r="K86" s="51"/>
+      <c r="L86" s="51"/>
+      <c r="M86" s="50"/>
     </row>
     <row r="87" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B87" s="49" t="s">
+      <c r="B87" s="45" t="s">
         <v>101</v>
       </c>
-      <c r="C87" s="50" t="s">
+      <c r="C87" s="46" t="s">
         <v>189</v>
       </c>
-      <c r="D87" s="50" t="s">
+      <c r="D87" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="E87" s="50" t="s">
+      <c r="E87" s="46" t="s">
         <v>190</v>
       </c>
-      <c r="F87" s="50" t="s">
+      <c r="F87" s="46" t="s">
         <v>191</v>
       </c>
-      <c r="G87" s="50" t="s">
+      <c r="G87" s="46" t="s">
         <v>192</v>
       </c>
-      <c r="H87" s="50" t="s">
+      <c r="H87" s="46" t="s">
         <v>193</v>
       </c>
-      <c r="I87" s="50" t="s">
+      <c r="I87" s="46" t="s">
         <v>194</v>
       </c>
-      <c r="J87" s="50" t="s">
+      <c r="J87" s="46" t="s">
         <v>195</v>
       </c>
-      <c r="K87" s="50"/>
-      <c r="L87" s="50"/>
-      <c r="M87" s="50"/>
-      <c r="N87" s="50"/>
-      <c r="O87" s="50"/>
-      <c r="P87" s="51"/>
-    </row>
-    <row r="88" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="B88" s="49" t="s">
+      <c r="K87" s="46"/>
+      <c r="L87" s="46"/>
+      <c r="M87" s="46"/>
+      <c r="N87" s="46"/>
+      <c r="O87" s="46"/>
+      <c r="P87" s="47"/>
+    </row>
+    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B88" s="45" t="s">
         <v>102</v>
       </c>
-      <c r="C88" s="50" t="s">
+      <c r="C88" s="46" t="s">
         <v>196</v>
       </c>
-      <c r="D88" s="50" t="s">
+      <c r="D88" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="E88" s="50" t="s">
+      <c r="E88" s="46" t="s">
         <v>197</v>
       </c>
-      <c r="F88" s="50" t="s">
+      <c r="F88" s="46" t="s">
         <v>198</v>
       </c>
-      <c r="G88" s="50" t="s">
+      <c r="G88" s="46" t="s">
         <v>199</v>
       </c>
-      <c r="H88" s="50" t="s">
+      <c r="H88" s="46" t="s">
         <v>200</v>
       </c>
-      <c r="I88" s="50" t="s">
+      <c r="I88" s="46" t="s">
         <v>201</v>
       </c>
-      <c r="J88" s="50" t="s">
+      <c r="J88" s="46" t="s">
         <v>202</v>
       </c>
-      <c r="K88" s="50"/>
-      <c r="L88" s="50"/>
-      <c r="M88" s="50"/>
-      <c r="N88" s="50"/>
-      <c r="O88" s="50"/>
-      <c r="P88" s="51"/>
-    </row>
-    <row r="89" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="B89" s="49" t="s">
+      <c r="K88" s="46"/>
+      <c r="L88" s="46"/>
+      <c r="M88" s="46"/>
+      <c r="N88" s="46"/>
+      <c r="O88" s="46"/>
+      <c r="P88" s="47"/>
+    </row>
+    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B89" s="45" t="s">
         <v>103</v>
       </c>
-      <c r="C89" s="50" t="s">
+      <c r="C89" s="46" t="s">
         <v>203</v>
       </c>
-      <c r="D89" s="50" t="s">
+      <c r="D89" s="46" t="s">
         <v>204</v>
       </c>
-      <c r="E89" s="50" t="s">
+      <c r="E89" s="46" t="s">
         <v>205</v>
       </c>
-      <c r="F89" s="50" t="s">
+      <c r="F89" s="46" t="s">
         <v>206</v>
       </c>
-      <c r="G89" s="50" t="s">
+      <c r="G89" s="46" t="s">
         <v>207</v>
       </c>
-      <c r="H89" s="50" t="s">
+      <c r="H89" s="46" t="s">
         <v>208</v>
       </c>
-      <c r="I89" s="50" t="s">
+      <c r="I89" s="46" t="s">
         <v>209</v>
       </c>
-      <c r="J89" s="50" t="s">
+      <c r="J89" s="46" t="s">
         <v>210</v>
       </c>
-      <c r="K89" s="50"/>
-      <c r="L89" s="50"/>
-      <c r="M89" s="50"/>
-      <c r="N89" s="50"/>
-      <c r="O89" s="50"/>
-      <c r="P89" s="51"/>
-    </row>
-    <row r="90" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="B90" s="49" t="s">
+      <c r="K89" s="46"/>
+      <c r="L89" s="46"/>
+      <c r="M89" s="46"/>
+      <c r="N89" s="46"/>
+      <c r="O89" s="46"/>
+      <c r="P89" s="47"/>
+    </row>
+    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B90" s="45" t="s">
         <v>104</v>
       </c>
-      <c r="C90" s="50" t="s">
+      <c r="C90" s="46" t="s">
         <v>211</v>
       </c>
-      <c r="D90" s="50" t="s">
+      <c r="D90" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="E90" s="50" t="s">
+      <c r="E90" s="46" t="s">
         <v>212</v>
       </c>
-      <c r="F90" s="50" t="s">
+      <c r="F90" s="46" t="s">
         <v>213</v>
       </c>
-      <c r="G90" s="50" t="s">
+      <c r="G90" s="46" t="s">
         <v>214</v>
       </c>
-      <c r="H90" s="50" t="s">
+      <c r="H90" s="46" t="s">
         <v>215</v>
       </c>
-      <c r="I90" s="50" t="s">
+      <c r="I90" s="46" t="s">
         <v>216</v>
       </c>
-      <c r="J90" s="50" t="s">
+      <c r="J90" s="46" t="s">
         <v>217</v>
       </c>
-      <c r="K90" s="50"/>
-      <c r="L90" s="50"/>
-      <c r="M90" s="50"/>
-      <c r="N90" s="50"/>
-      <c r="O90" s="50"/>
-      <c r="P90" s="51"/>
-    </row>
-    <row r="91" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="B91" s="49" t="s">
+      <c r="K90" s="46"/>
+      <c r="L90" s="46"/>
+      <c r="M90" s="46"/>
+      <c r="N90" s="46"/>
+      <c r="O90" s="46"/>
+      <c r="P90" s="47"/>
+    </row>
+    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B91" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="C91" s="50" t="s">
+      <c r="C91" s="46" t="s">
         <v>218</v>
       </c>
-      <c r="D91" s="50" t="s">
+      <c r="D91" s="46" t="s">
         <v>219</v>
       </c>
-      <c r="E91" s="50" t="s">
+      <c r="E91" s="46" t="s">
         <v>220</v>
       </c>
-      <c r="F91" s="50" t="s">
+      <c r="F91" s="46" t="s">
         <v>221</v>
       </c>
-      <c r="G91" s="50" t="s">
+      <c r="G91" s="46" t="s">
         <v>222</v>
       </c>
-      <c r="H91" s="50" t="s">
+      <c r="H91" s="46" t="s">
         <v>223</v>
       </c>
-      <c r="I91" s="50" t="s">
+      <c r="I91" s="46" t="s">
         <v>224</v>
       </c>
-      <c r="J91" s="50" t="s">
+      <c r="J91" s="46" t="s">
         <v>225</v>
       </c>
-      <c r="K91" s="50"/>
-      <c r="L91" s="50"/>
-      <c r="M91" s="50"/>
-      <c r="N91" s="50"/>
-      <c r="O91" s="50"/>
-      <c r="P91" s="51"/>
-    </row>
-    <row r="92" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="B92" s="49" t="s">
+      <c r="K91" s="46"/>
+      <c r="L91" s="46"/>
+      <c r="M91" s="46"/>
+      <c r="N91" s="46"/>
+      <c r="O91" s="46"/>
+      <c r="P91" s="47"/>
+    </row>
+    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B92" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="C92" s="50" t="s">
+      <c r="C92" s="46" t="s">
         <v>226</v>
       </c>
-      <c r="D92" s="50" t="s">
+      <c r="D92" s="46" t="s">
         <v>227</v>
       </c>
-      <c r="E92" s="50" t="s">
+      <c r="E92" s="46" t="s">
         <v>228</v>
       </c>
-      <c r="F92" s="50" t="s">
+      <c r="F92" s="46" t="s">
         <v>229</v>
       </c>
-      <c r="G92" s="50" t="s">
+      <c r="G92" s="46" t="s">
         <v>230</v>
       </c>
-      <c r="H92" s="50" t="s">
+      <c r="H92" s="46" t="s">
         <v>231</v>
       </c>
-      <c r="I92" s="50" t="s">
+      <c r="I92" s="46" t="s">
         <v>232</v>
       </c>
-      <c r="J92" s="50" t="s">
+      <c r="J92" s="46" t="s">
         <v>233</v>
       </c>
-      <c r="K92" s="50"/>
-      <c r="L92" s="50"/>
-      <c r="M92" s="50"/>
-      <c r="N92" s="50"/>
-      <c r="O92" s="50"/>
-      <c r="P92" s="51"/>
-    </row>
-    <row r="93" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="B93" s="49" t="s">
+      <c r="K92" s="46"/>
+      <c r="L92" s="46"/>
+      <c r="M92" s="46"/>
+      <c r="N92" s="46"/>
+      <c r="O92" s="46"/>
+      <c r="P92" s="47"/>
+    </row>
+    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B93" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="C93" s="50" t="s">
+      <c r="C93" s="46" t="s">
         <v>234</v>
       </c>
-      <c r="D93" s="50" t="s">
+      <c r="D93" s="46" t="s">
         <v>235</v>
       </c>
-      <c r="E93" s="50" t="s">
+      <c r="E93" s="46" t="s">
         <v>236</v>
       </c>
-      <c r="F93" s="50" t="s">
+      <c r="F93" s="46" t="s">
         <v>237</v>
       </c>
-      <c r="G93" s="50" t="s">
+      <c r="G93" s="46" t="s">
         <v>238</v>
       </c>
-      <c r="H93" s="50" t="s">
+      <c r="H93" s="46" t="s">
         <v>239</v>
       </c>
-      <c r="I93" s="50" t="s">
+      <c r="I93" s="46" t="s">
         <v>240</v>
       </c>
-      <c r="J93" s="50" t="s">
+      <c r="J93" s="46" t="s">
         <v>241</v>
       </c>
-      <c r="K93" s="50"/>
-      <c r="L93" s="50"/>
-      <c r="M93" s="50"/>
-      <c r="N93" s="50"/>
-      <c r="O93" s="50"/>
-      <c r="P93" s="51"/>
-    </row>
-    <row r="94" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="B94" s="49" t="s">
+      <c r="K93" s="46"/>
+      <c r="L93" s="46"/>
+      <c r="M93" s="46"/>
+      <c r="N93" s="46"/>
+      <c r="O93" s="46"/>
+      <c r="P93" s="47"/>
+    </row>
+    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B94" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="C94" s="50" t="s">
+      <c r="C94" s="46" t="s">
         <v>242</v>
       </c>
-      <c r="D94" s="50" t="s">
+      <c r="D94" s="46" t="s">
         <v>243</v>
       </c>
-      <c r="E94" s="50" t="s">
+      <c r="E94" s="46" t="s">
         <v>244</v>
       </c>
-      <c r="F94" s="50" t="s">
+      <c r="F94" s="46" t="s">
         <v>245</v>
       </c>
-      <c r="G94" s="50" t="s">
+      <c r="G94" s="46" t="s">
         <v>180</v>
       </c>
-      <c r="H94" s="50" t="s">
+      <c r="H94" s="46" t="s">
         <v>246</v>
       </c>
-      <c r="I94" s="50" t="s">
+      <c r="I94" s="46" t="s">
         <v>247</v>
       </c>
-      <c r="J94" s="50" t="s">
+      <c r="J94" s="46" t="s">
         <v>248</v>
       </c>
-      <c r="K94" s="50"/>
-      <c r="L94" s="50"/>
-      <c r="M94" s="50"/>
-      <c r="N94" s="50"/>
-      <c r="O94" s="50"/>
-      <c r="P94" s="51"/>
-    </row>
-    <row r="95" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="B95" s="49" t="s">
+      <c r="K94" s="46"/>
+      <c r="L94" s="46"/>
+      <c r="M94" s="46"/>
+      <c r="N94" s="46"/>
+      <c r="O94" s="46"/>
+      <c r="P94" s="47"/>
+    </row>
+    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B95" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="C95" s="50" t="s">
+      <c r="C95" s="46" t="s">
         <v>262</v>
       </c>
-      <c r="D95" s="50" t="s">
+      <c r="D95" s="46" t="s">
         <v>263</v>
       </c>
-      <c r="E95" s="50" t="s">
+      <c r="E95" s="46" t="s">
         <v>264</v>
       </c>
-      <c r="F95" s="50" t="s">
+      <c r="F95" s="46" t="s">
         <v>265</v>
       </c>
-      <c r="G95" s="50" t="s">
+      <c r="G95" s="46" t="s">
         <v>266</v>
       </c>
-      <c r="H95" s="50" t="s">
+      <c r="H95" s="46" t="s">
         <v>267</v>
       </c>
-      <c r="I95" s="50" t="s">
+      <c r="I95" s="46" t="s">
         <v>268</v>
       </c>
-      <c r="J95" s="50" t="s">
+      <c r="J95" s="46" t="s">
         <v>269</v>
       </c>
-      <c r="K95" s="50"/>
-      <c r="L95" s="50"/>
-      <c r="M95" s="51"/>
-    </row>
-    <row r="96" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="B96" s="49" t="s">
+      <c r="K95" s="46"/>
+      <c r="L95" s="46"/>
+      <c r="M95" s="47"/>
+    </row>
+    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B96" s="45" t="s">
         <v>109</v>
       </c>
-      <c r="C96" s="50" t="s">
+      <c r="C96" s="46" t="s">
         <v>270</v>
       </c>
-      <c r="D96" s="50" t="s">
+      <c r="D96" s="46" t="s">
         <v>271</v>
       </c>
-      <c r="E96" s="50" t="s">
+      <c r="E96" s="46" t="s">
         <v>272</v>
       </c>
-      <c r="F96" s="50" t="s">
+      <c r="F96" s="46" t="s">
         <v>273</v>
       </c>
-      <c r="G96" s="50" t="s">
+      <c r="G96" s="46" t="s">
         <v>274</v>
       </c>
-      <c r="H96" s="50" t="s">
+      <c r="H96" s="46" t="s">
         <v>275</v>
       </c>
-      <c r="I96" s="50" t="s">
+      <c r="I96" s="46" t="s">
         <v>276</v>
       </c>
-      <c r="J96" s="50" t="s">
+      <c r="J96" s="46" t="s">
         <v>277</v>
       </c>
-      <c r="K96" s="50"/>
-      <c r="L96" s="50"/>
-      <c r="M96" s="51"/>
-    </row>
-    <row r="97" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B97" s="49" t="s">
+      <c r="K96" s="46"/>
+      <c r="L96" s="46"/>
+      <c r="M96" s="47"/>
+    </row>
+    <row r="97" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B97" s="45" t="s">
         <v>49</v>
       </c>
-      <c r="C97" s="50" t="s">
+      <c r="C97" s="46" t="s">
         <v>278</v>
       </c>
-      <c r="D97" s="50" t="s">
+      <c r="D97" s="46" t="s">
         <v>279</v>
       </c>
-      <c r="E97" s="50" t="s">
+      <c r="E97" s="46" t="s">
         <v>280</v>
       </c>
-      <c r="F97" s="50" t="s">
+      <c r="F97" s="46" t="s">
         <v>281</v>
       </c>
-      <c r="G97" s="50" t="s">
+      <c r="G97" s="46" t="s">
         <v>282</v>
       </c>
-      <c r="H97" s="50" t="s">
+      <c r="H97" s="46" t="s">
         <v>283</v>
       </c>
-      <c r="I97" s="50" t="s">
+      <c r="I97" s="46" t="s">
         <v>284</v>
       </c>
-      <c r="J97" s="50" t="s">
+      <c r="J97" s="46" t="s">
         <v>285</v>
       </c>
-      <c r="K97" s="50"/>
-      <c r="L97" s="50"/>
-      <c r="M97" s="51"/>
-    </row>
-    <row r="98" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B98" s="49" t="s">
+      <c r="K97" s="46"/>
+      <c r="L97" s="46"/>
+      <c r="M97" s="47"/>
+    </row>
+    <row r="98" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B98" s="45" t="s">
         <v>147</v>
       </c>
-      <c r="C98" s="50" t="s">
+      <c r="C98" s="46" t="s">
         <v>286</v>
       </c>
-      <c r="D98" s="50" t="s">
+      <c r="D98" s="46" t="s">
         <v>287</v>
       </c>
-      <c r="E98" s="50" t="s">
+      <c r="E98" s="46" t="s">
         <v>288</v>
       </c>
-      <c r="F98" s="50" t="s">
+      <c r="F98" s="46" t="s">
         <v>289</v>
       </c>
-      <c r="G98" s="50" t="s">
+      <c r="G98" s="46" t="s">
         <v>290</v>
       </c>
-      <c r="H98" s="50" t="s">
+      <c r="H98" s="46" t="s">
         <v>291</v>
       </c>
-      <c r="I98" s="50" t="s">
+      <c r="I98" s="46" t="s">
         <v>292</v>
       </c>
-      <c r="J98" s="50" t="s">
+      <c r="J98" s="46" t="s">
         <v>293</v>
       </c>
-      <c r="K98" s="50"/>
-      <c r="L98" s="50"/>
-      <c r="M98" s="51"/>
-    </row>
-    <row r="99" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B99" s="49" t="s">
+      <c r="K98" s="46"/>
+      <c r="L98" s="46"/>
+      <c r="M98" s="47"/>
+    </row>
+    <row r="99" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B99" s="45" t="s">
         <v>108</v>
       </c>
-      <c r="C99" s="50" t="s">
+      <c r="C99" s="46" t="s">
         <v>294</v>
       </c>
-      <c r="D99" s="50" t="s">
+      <c r="D99" s="46" t="s">
         <v>295</v>
       </c>
-      <c r="E99" s="50" t="s">
+      <c r="E99" s="46" t="s">
         <v>296</v>
       </c>
-      <c r="F99" s="50" t="s">
+      <c r="F99" s="46" t="s">
         <v>297</v>
       </c>
-      <c r="G99" s="50" t="s">
+      <c r="G99" s="46" t="s">
         <v>298</v>
       </c>
-      <c r="H99" s="50" t="s">
+      <c r="H99" s="46" t="s">
         <v>299</v>
       </c>
-      <c r="I99" s="50" t="s">
+      <c r="I99" s="46" t="s">
         <v>300</v>
       </c>
-      <c r="J99" s="50" t="s">
+      <c r="J99" s="46" t="s">
         <v>301</v>
       </c>
-      <c r="K99" s="50"/>
-      <c r="L99" s="50"/>
-      <c r="M99" s="51"/>
-    </row>
-    <row r="100" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B100" s="49" t="s">
+      <c r="K99" s="46"/>
+      <c r="L99" s="46"/>
+      <c r="M99" s="47"/>
+    </row>
+    <row r="100" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B100" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="C100" s="50" t="s">
+      <c r="C100" s="46" t="s">
         <v>302</v>
       </c>
-      <c r="D100" s="50" t="s">
+      <c r="D100" s="46" t="s">
         <v>303</v>
       </c>
-      <c r="E100" s="50" t="s">
+      <c r="E100" s="46" t="s">
         <v>304</v>
       </c>
-      <c r="F100" s="50" t="s">
+      <c r="F100" s="46" t="s">
         <v>305</v>
       </c>
-      <c r="G100" s="50" t="s">
+      <c r="G100" s="46" t="s">
         <v>306</v>
       </c>
-      <c r="H100" s="50" t="s">
+      <c r="H100" s="46" t="s">
         <v>307</v>
       </c>
-      <c r="I100" s="50" t="s">
+      <c r="I100" s="46" t="s">
         <v>308</v>
       </c>
-      <c r="J100" s="50" t="s">
+      <c r="J100" s="46" t="s">
         <v>309</v>
       </c>
-      <c r="K100" s="50"/>
-      <c r="L100" s="50"/>
-      <c r="M100" s="51"/>
-    </row>
-    <row r="101" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B101" s="49" t="s">
+      <c r="K100" s="46"/>
+      <c r="L100" s="46"/>
+      <c r="M100" s="47"/>
+    </row>
+    <row r="101" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B101" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="C101" s="50" t="s">
+      <c r="C101" s="46" t="s">
         <v>310</v>
       </c>
-      <c r="D101" s="50" t="s">
+      <c r="D101" s="46" t="s">
         <v>311</v>
       </c>
-      <c r="E101" s="50" t="s">
+      <c r="E101" s="46" t="s">
         <v>312</v>
       </c>
-      <c r="F101" s="50" t="s">
+      <c r="F101" s="46" t="s">
         <v>313</v>
       </c>
-      <c r="G101" s="50" t="s">
+      <c r="G101" s="46" t="s">
         <v>314</v>
       </c>
-      <c r="H101" s="50" t="s">
+      <c r="H101" s="46" t="s">
         <v>315</v>
       </c>
-      <c r="I101" s="50" t="s">
+      <c r="I101" s="46" t="s">
         <v>316</v>
       </c>
-      <c r="J101" s="50" t="s">
+      <c r="J101" s="46" t="s">
         <v>317</v>
       </c>
-      <c r="K101" s="50"/>
-      <c r="L101" s="50"/>
-      <c r="M101" s="51"/>
-    </row>
-    <row r="102" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B102" s="49" t="s">
+      <c r="K101" s="46"/>
+      <c r="L101" s="46"/>
+      <c r="M101" s="47"/>
+    </row>
+    <row r="102" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B102" s="45" t="s">
         <v>105</v>
       </c>
-      <c r="C102" s="50" t="s">
+      <c r="C102" s="46" t="s">
         <v>318</v>
       </c>
-      <c r="D102" s="50" t="s">
+      <c r="D102" s="46" t="s">
         <v>319</v>
       </c>
-      <c r="E102" s="50" t="s">
+      <c r="E102" s="46" t="s">
         <v>320</v>
       </c>
-      <c r="F102" s="50" t="s">
+      <c r="F102" s="46" t="s">
         <v>321</v>
       </c>
-      <c r="G102" s="50" t="s">
+      <c r="G102" s="46" t="s">
         <v>322</v>
       </c>
-      <c r="H102" s="50" t="s">
+      <c r="H102" s="46" t="s">
         <v>323</v>
       </c>
-      <c r="I102" s="50" t="s">
+      <c r="I102" s="46" t="s">
         <v>324</v>
       </c>
-      <c r="J102" s="50" t="s">
+      <c r="J102" s="46" t="s">
         <v>325</v>
       </c>
-      <c r="K102" s="50"/>
-      <c r="L102" s="50"/>
-      <c r="M102" s="51"/>
-    </row>
-    <row r="103" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B103" s="49" t="s">
+      <c r="K102" s="46"/>
+      <c r="L102" s="46"/>
+      <c r="M102" s="47"/>
+    </row>
+    <row r="103" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B103" s="45" t="s">
         <v>146</v>
       </c>
-      <c r="C103" s="50" t="s">
+      <c r="C103" s="46" t="s">
         <v>326</v>
       </c>
-      <c r="D103" s="50" t="s">
+      <c r="D103" s="46" t="s">
         <v>327</v>
       </c>
-      <c r="E103" s="50" t="s">
+      <c r="E103" s="46" t="s">
         <v>328</v>
       </c>
-      <c r="F103" s="50" t="s">
+      <c r="F103" s="46" t="s">
         <v>329</v>
       </c>
-      <c r="G103" s="50" t="s">
+      <c r="G103" s="46" t="s">
         <v>330</v>
       </c>
-      <c r="H103" s="50" t="s">
+      <c r="H103" s="46" t="s">
         <v>331</v>
       </c>
-      <c r="I103" s="50" t="s">
+      <c r="I103" s="46" t="s">
         <v>332</v>
       </c>
-      <c r="J103" s="50" t="s">
+      <c r="J103" s="46" t="s">
         <v>333</v>
       </c>
-      <c r="K103" s="50"/>
-      <c r="L103" s="50"/>
-      <c r="M103" s="51"/>
-    </row>
-    <row r="104" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B104" s="49" t="s">
+      <c r="K103" s="46"/>
+      <c r="L103" s="46"/>
+      <c r="M103" s="47"/>
+    </row>
+    <row r="104" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B104" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="C104" s="50" t="s">
+      <c r="C104" s="46" t="s">
         <v>334</v>
       </c>
-      <c r="D104" s="50" t="s">
+      <c r="D104" s="46" t="s">
         <v>335</v>
       </c>
-      <c r="E104" s="50" t="s">
+      <c r="E104" s="46" t="s">
         <v>336</v>
       </c>
-      <c r="F104" s="50" t="s">
+      <c r="F104" s="46" t="s">
         <v>337</v>
       </c>
-      <c r="G104" s="50" t="s">
+      <c r="G104" s="46" t="s">
         <v>338</v>
       </c>
-      <c r="H104" s="50" t="s">
+      <c r="H104" s="46" t="s">
         <v>339</v>
       </c>
-      <c r="I104" s="50" t="s">
+      <c r="I104" s="46" t="s">
         <v>340</v>
       </c>
-      <c r="J104" s="50" t="s">
+      <c r="J104" s="46" t="s">
         <v>341</v>
       </c>
-      <c r="K104" s="50"/>
-      <c r="L104" s="50"/>
-      <c r="M104" s="51"/>
-    </row>
-    <row r="105" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B105" s="49" t="s">
+      <c r="K104" s="46"/>
+      <c r="L104" s="46"/>
+      <c r="M104" s="47"/>
+    </row>
+    <row r="105" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B105" s="45" t="s">
         <v>143</v>
       </c>
-      <c r="C105" s="50" t="s">
+      <c r="C105" s="46" t="s">
         <v>342</v>
       </c>
-      <c r="D105" s="50" t="s">
+      <c r="D105" s="46" t="s">
         <v>343</v>
       </c>
-      <c r="E105" s="50" t="s">
+      <c r="E105" s="46" t="s">
         <v>344</v>
       </c>
-      <c r="F105" s="50" t="s">
+      <c r="F105" s="46" t="s">
         <v>345</v>
       </c>
-      <c r="G105" s="50" t="s">
+      <c r="G105" s="46" t="s">
         <v>346</v>
       </c>
-      <c r="H105" s="50" t="s">
+      <c r="H105" s="46" t="s">
         <v>347</v>
       </c>
-      <c r="I105" s="50" t="s">
+      <c r="I105" s="46" t="s">
         <v>348</v>
       </c>
-      <c r="J105" s="50" t="s">
+      <c r="J105" s="46" t="s">
         <v>349</v>
       </c>
-      <c r="K105" s="50"/>
-      <c r="L105" s="50"/>
-      <c r="M105" s="51"/>
-    </row>
-    <row r="106" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B106" s="49" t="s">
+      <c r="K105" s="46"/>
+      <c r="L105" s="46"/>
+      <c r="M105" s="47"/>
+    </row>
+    <row r="106" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B106" s="45" t="s">
         <v>151</v>
       </c>
-      <c r="C106" s="50" t="s">
+      <c r="C106" s="46" t="s">
         <v>350</v>
       </c>
-      <c r="D106" s="50" t="s">
+      <c r="D106" s="46" t="s">
         <v>351</v>
       </c>
-      <c r="E106" s="50" t="s">
+      <c r="E106" s="46" t="s">
         <v>352</v>
       </c>
-      <c r="F106" s="50" t="s">
+      <c r="F106" s="46" t="s">
         <v>353</v>
       </c>
-      <c r="G106" s="50" t="s">
+      <c r="G106" s="46" t="s">
         <v>354</v>
       </c>
-      <c r="H106" s="50" t="s">
+      <c r="H106" s="46" t="s">
         <v>355</v>
       </c>
-      <c r="I106" s="50" t="s">
+      <c r="I106" s="46" t="s">
         <v>356</v>
       </c>
-      <c r="J106" s="50" t="s">
+      <c r="J106" s="46" t="s">
         <v>357</v>
       </c>
-      <c r="K106" s="50"/>
-      <c r="L106" s="50"/>
-      <c r="M106" s="51"/>
-    </row>
-    <row r="107" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B107" s="49" t="s">
+      <c r="K106" s="46"/>
+      <c r="L106" s="46"/>
+      <c r="M106" s="47"/>
+    </row>
+    <row r="107" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B107" s="45" t="s">
         <v>165</v>
       </c>
-      <c r="C107" s="50" t="s">
+      <c r="C107" s="46" t="s">
         <v>358</v>
       </c>
-      <c r="D107" s="50" t="s">
+      <c r="D107" s="46" t="s">
         <v>359</v>
       </c>
-      <c r="E107" s="50" t="s">
+      <c r="E107" s="46" t="s">
         <v>360</v>
       </c>
-      <c r="F107" s="50" t="s">
+      <c r="F107" s="46" t="s">
         <v>361</v>
       </c>
-      <c r="G107" s="50" t="s">
+      <c r="G107" s="46" t="s">
         <v>362</v>
       </c>
-      <c r="H107" s="50" t="s">
+      <c r="H107" s="46" t="s">
         <v>363</v>
       </c>
-      <c r="I107" s="50" t="s">
+      <c r="I107" s="46" t="s">
         <v>364</v>
       </c>
-      <c r="J107" s="50" t="s">
+      <c r="J107" s="46" t="s">
         <v>365</v>
       </c>
-      <c r="K107" s="50"/>
-      <c r="L107" s="50"/>
-      <c r="M107" s="51"/>
-    </row>
-    <row r="108" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B108" s="49" t="s">
+      <c r="K107" s="46"/>
+      <c r="L107" s="46"/>
+      <c r="M107" s="47"/>
+    </row>
+    <row r="108" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B108" s="45" t="s">
         <v>128</v>
       </c>
-      <c r="C108" s="50" t="s">
+      <c r="C108" s="46" t="s">
         <v>366</v>
       </c>
-      <c r="D108" s="50" t="s">
+      <c r="D108" s="46" t="s">
         <v>367</v>
       </c>
-      <c r="E108" s="50" t="s">
+      <c r="E108" s="46" t="s">
         <v>368</v>
       </c>
-      <c r="F108" s="50" t="s">
+      <c r="F108" s="46" t="s">
         <v>369</v>
       </c>
-      <c r="G108" s="50" t="s">
+      <c r="G108" s="46" t="s">
         <v>370</v>
       </c>
-      <c r="H108" s="50" t="s">
+      <c r="H108" s="46" t="s">
         <v>371</v>
       </c>
-      <c r="I108" s="50" t="s">
+      <c r="I108" s="46" t="s">
         <v>372</v>
       </c>
-      <c r="J108" s="50" t="s">
+      <c r="J108" s="46" t="s">
         <v>373</v>
       </c>
-      <c r="K108" s="50"/>
-      <c r="L108" s="50"/>
-      <c r="M108" s="51"/>
-    </row>
-    <row r="109" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B109" s="49" t="s">
+      <c r="K108" s="46"/>
+      <c r="L108" s="46"/>
+      <c r="M108" s="47"/>
+    </row>
+    <row r="109" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B109" s="45" t="s">
         <v>161</v>
       </c>
-      <c r="C109" s="50" t="s">
+      <c r="C109" s="46" t="s">
         <v>374</v>
       </c>
-      <c r="D109" s="50" t="s">
+      <c r="D109" s="46" t="s">
         <v>375</v>
       </c>
-      <c r="E109" s="50" t="s">
+      <c r="E109" s="46" t="s">
         <v>376</v>
       </c>
-      <c r="F109" s="50" t="s">
+      <c r="F109" s="46" t="s">
         <v>377</v>
       </c>
-      <c r="G109" s="50" t="s">
+      <c r="G109" s="46" t="s">
         <v>378</v>
       </c>
-      <c r="H109" s="50" t="s">
+      <c r="H109" s="46" t="s">
         <v>379</v>
       </c>
-      <c r="I109" s="50" t="s">
+      <c r="I109" s="46" t="s">
         <v>380</v>
       </c>
-      <c r="J109" s="50" t="s">
+      <c r="J109" s="46" t="s">
         <v>381</v>
       </c>
-      <c r="K109" s="50"/>
-      <c r="L109" s="50"/>
-      <c r="M109" s="51"/>
-    </row>
-    <row r="110" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B110" s="49" t="s">
+      <c r="K109" s="46"/>
+      <c r="L109" s="46"/>
+      <c r="M109" s="47"/>
+    </row>
+    <row r="110" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B110" s="45" t="s">
         <v>129</v>
       </c>
-      <c r="C110" s="50" t="s">
+      <c r="C110" s="46" t="s">
         <v>382</v>
       </c>
-      <c r="D110" s="50" t="s">
+      <c r="D110" s="46" t="s">
         <v>383</v>
       </c>
-      <c r="E110" s="50" t="s">
+      <c r="E110" s="46" t="s">
         <v>384</v>
       </c>
-      <c r="F110" s="50" t="s">
+      <c r="F110" s="46" t="s">
         <v>385</v>
       </c>
-      <c r="G110" s="50" t="s">
+      <c r="G110" s="46" t="s">
         <v>386</v>
       </c>
-      <c r="H110" s="50" t="s">
+      <c r="H110" s="46" t="s">
         <v>387</v>
       </c>
-      <c r="I110" s="50" t="s">
+      <c r="I110" s="46" t="s">
         <v>388</v>
       </c>
-      <c r="J110" s="50" t="s">
+      <c r="J110" s="46" t="s">
         <v>389</v>
       </c>
-      <c r="K110" s="50"/>
-      <c r="L110" s="50"/>
-      <c r="M110" s="51"/>
-    </row>
-    <row r="111" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B111" s="49" t="s">
+      <c r="K110" s="46"/>
+      <c r="L110" s="46"/>
+      <c r="M110" s="47"/>
+    </row>
+    <row r="111" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B111" s="45" t="s">
         <v>148</v>
       </c>
-      <c r="C111" s="50" t="s">
+      <c r="C111" s="46" t="s">
         <v>390</v>
       </c>
-      <c r="D111" s="50" t="s">
+      <c r="D111" s="46" t="s">
         <v>391</v>
       </c>
-      <c r="E111" s="50" t="s">
+      <c r="E111" s="46" t="s">
         <v>392</v>
       </c>
-      <c r="F111" s="50" t="s">
+      <c r="F111" s="46" t="s">
         <v>393</v>
       </c>
-      <c r="G111" s="50" t="s">
+      <c r="G111" s="46" t="s">
         <v>394</v>
       </c>
-      <c r="H111" s="50" t="s">
+      <c r="H111" s="46" t="s">
         <v>395</v>
       </c>
-      <c r="I111" s="50" t="s">
+      <c r="I111" s="46" t="s">
         <v>396</v>
       </c>
-      <c r="J111" s="50" t="s">
+      <c r="J111" s="46" t="s">
         <v>397</v>
       </c>
-      <c r="K111" s="50"/>
-      <c r="L111" s="50"/>
-      <c r="M111" s="51"/>
-    </row>
-    <row r="112" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B112" s="49" t="s">
+      <c r="K111" s="46"/>
+      <c r="L111" s="46"/>
+      <c r="M111" s="47"/>
+    </row>
+    <row r="112" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B112" s="45" t="s">
         <v>155</v>
       </c>
-      <c r="C112" s="50" t="s">
+      <c r="C112" s="46" t="s">
         <v>398</v>
       </c>
-      <c r="D112" s="50" t="s">
+      <c r="D112" s="46" t="s">
         <v>399</v>
       </c>
-      <c r="E112" s="50" t="s">
+      <c r="E112" s="46" t="s">
         <v>400</v>
       </c>
-      <c r="F112" s="50" t="s">
+      <c r="F112" s="46" t="s">
         <v>401</v>
       </c>
-      <c r="G112" s="50" t="s">
+      <c r="G112" s="46" t="s">
         <v>402</v>
       </c>
-      <c r="H112" s="50" t="s">
+      <c r="H112" s="46" t="s">
         <v>403</v>
       </c>
-      <c r="I112" s="50" t="s">
+      <c r="I112" s="46" t="s">
         <v>404</v>
       </c>
-      <c r="J112" s="50" t="s">
+      <c r="J112" s="46" t="s">
         <v>405</v>
       </c>
-      <c r="K112" s="50"/>
-      <c r="L112" s="50"/>
-      <c r="M112" s="51"/>
-    </row>
-    <row r="113" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B113" s="49" t="s">
+      <c r="K112" s="46"/>
+      <c r="L112" s="46"/>
+      <c r="M112" s="47"/>
+    </row>
+    <row r="113" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B113" s="45" t="s">
         <v>121</v>
       </c>
-      <c r="C113" s="50" t="s">
+      <c r="C113" s="46" t="s">
         <v>406</v>
       </c>
-      <c r="D113" s="50" t="s">
+      <c r="D113" s="46" t="s">
         <v>407</v>
       </c>
-      <c r="E113" s="50" t="s">
+      <c r="E113" s="46" t="s">
         <v>408</v>
       </c>
-      <c r="F113" s="50" t="s">
+      <c r="F113" s="46" t="s">
         <v>409</v>
       </c>
-      <c r="G113" s="50" t="s">
+      <c r="G113" s="46" t="s">
         <v>410</v>
       </c>
-      <c r="H113" s="50" t="s">
+      <c r="H113" s="46" t="s">
         <v>411</v>
       </c>
-      <c r="I113" s="50" t="s">
+      <c r="I113" s="46" t="s">
         <v>412</v>
       </c>
-      <c r="J113" s="50" t="s">
+      <c r="J113" s="46" t="s">
         <v>413</v>
       </c>
-      <c r="K113" s="50"/>
-      <c r="L113" s="50"/>
-      <c r="M113" s="51"/>
-    </row>
-    <row r="114" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B114" s="49" t="s">
+      <c r="K113" s="46"/>
+      <c r="L113" s="46"/>
+      <c r="M113" s="47"/>
+    </row>
+    <row r="114" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B114" s="45" t="s">
         <v>134</v>
       </c>
-      <c r="C114" s="50" t="s">
+      <c r="C114" s="46" t="s">
         <v>414</v>
       </c>
-      <c r="D114" s="50" t="s">
+      <c r="D114" s="46" t="s">
         <v>415</v>
       </c>
-      <c r="E114" s="50" t="s">
+      <c r="E114" s="46" t="s">
         <v>416</v>
       </c>
-      <c r="F114" s="50" t="s">
+      <c r="F114" s="46" t="s">
         <v>417</v>
       </c>
-      <c r="G114" s="50" t="s">
+      <c r="G114" s="46" t="s">
         <v>418</v>
       </c>
-      <c r="H114" s="50" t="s">
+      <c r="H114" s="46" t="s">
         <v>419</v>
       </c>
-      <c r="I114" s="50" t="s">
+      <c r="I114" s="46" t="s">
         <v>420</v>
       </c>
-      <c r="J114" s="50" t="s">
+      <c r="J114" s="46" t="s">
         <v>421</v>
       </c>
-      <c r="K114" s="50"/>
-      <c r="L114" s="50"/>
-      <c r="M114" s="51"/>
-    </row>
-    <row r="115" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B115" s="49" t="s">
+      <c r="K114" s="46"/>
+      <c r="L114" s="46"/>
+      <c r="M114" s="47"/>
+    </row>
+    <row r="115" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B115" s="45" t="s">
         <v>122</v>
       </c>
-      <c r="C115" s="50" t="s">
+      <c r="C115" s="46" t="s">
         <v>422</v>
       </c>
-      <c r="D115" s="50" t="s">
+      <c r="D115" s="46" t="s">
         <v>423</v>
       </c>
-      <c r="E115" s="50" t="s">
+      <c r="E115" s="46" t="s">
         <v>424</v>
       </c>
-      <c r="F115" s="50" t="s">
+      <c r="F115" s="46" t="s">
         <v>425</v>
       </c>
-      <c r="G115" s="50" t="s">
+      <c r="G115" s="46" t="s">
         <v>426</v>
       </c>
-      <c r="H115" s="50" t="s">
+      <c r="H115" s="46" t="s">
         <v>427</v>
       </c>
-      <c r="I115" s="50" t="s">
+      <c r="I115" s="46" t="s">
         <v>428</v>
       </c>
-      <c r="J115" s="50" t="s">
+      <c r="J115" s="46" t="s">
         <v>429</v>
       </c>
-      <c r="K115" s="50"/>
-      <c r="L115" s="50"/>
-      <c r="M115" s="51"/>
-    </row>
-    <row r="116" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B116" s="49" t="s">
+      <c r="K115" s="46"/>
+      <c r="L115" s="46"/>
+      <c r="M115" s="47"/>
+    </row>
+    <row r="116" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B116" s="45" t="s">
         <v>120</v>
       </c>
-      <c r="C116" s="50" t="s">
+      <c r="C116" s="46" t="s">
         <v>430</v>
       </c>
-      <c r="D116" s="50" t="s">
+      <c r="D116" s="46" t="s">
         <v>431</v>
       </c>
-      <c r="E116" s="50" t="s">
+      <c r="E116" s="46" t="s">
         <v>432</v>
       </c>
-      <c r="F116" s="50" t="s">
+      <c r="F116" s="46" t="s">
         <v>433</v>
       </c>
-      <c r="G116" s="50" t="s">
+      <c r="G116" s="46" t="s">
         <v>434</v>
       </c>
-      <c r="H116" s="50" t="s">
+      <c r="H116" s="46" t="s">
         <v>435</v>
       </c>
-      <c r="I116" s="50" t="s">
+      <c r="I116" s="46" t="s">
         <v>436</v>
       </c>
-      <c r="J116" s="50" t="s">
+      <c r="J116" s="46" t="s">
         <v>437</v>
       </c>
-      <c r="K116" s="50"/>
-      <c r="L116" s="50"/>
-      <c r="M116" s="51"/>
-    </row>
-    <row r="117" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B117" s="49" t="s">
+      <c r="K116" s="46"/>
+      <c r="L116" s="46"/>
+      <c r="M116" s="47"/>
+    </row>
+    <row r="117" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B117" s="45" t="s">
         <v>149</v>
       </c>
-      <c r="C117" s="50" t="s">
+      <c r="C117" s="46" t="s">
         <v>438</v>
       </c>
-      <c r="D117" s="50" t="s">
+      <c r="D117" s="46" t="s">
         <v>439</v>
       </c>
-      <c r="E117" s="50" t="s">
+      <c r="E117" s="46" t="s">
         <v>440</v>
       </c>
-      <c r="F117" s="50" t="s">
+      <c r="F117" s="46" t="s">
         <v>441</v>
       </c>
-      <c r="G117" s="50" t="s">
+      <c r="G117" s="46" t="s">
         <v>442</v>
       </c>
-      <c r="H117" s="50" t="s">
+      <c r="H117" s="46" t="s">
         <v>443</v>
       </c>
-      <c r="I117" s="50" t="s">
+      <c r="I117" s="46" t="s">
         <v>444</v>
       </c>
-      <c r="J117" s="50" t="s">
+      <c r="J117" s="46" t="s">
         <v>445</v>
       </c>
-      <c r="K117" s="50"/>
-      <c r="L117" s="50"/>
-      <c r="M117" s="51"/>
-    </row>
-    <row r="118" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B118" s="49" t="s">
+      <c r="K117" s="46"/>
+      <c r="L117" s="46"/>
+      <c r="M117" s="47"/>
+    </row>
+    <row r="118" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B118" s="45" t="s">
         <v>138</v>
       </c>
-      <c r="C118" s="50" t="s">
+      <c r="C118" s="46" t="s">
         <v>446</v>
       </c>
-      <c r="D118" s="50" t="s">
+      <c r="D118" s="46" t="s">
         <v>447</v>
       </c>
-      <c r="E118" s="50" t="s">
+      <c r="E118" s="46" t="s">
         <v>448</v>
       </c>
-      <c r="F118" s="50" t="s">
+      <c r="F118" s="46" t="s">
         <v>449</v>
       </c>
-      <c r="G118" s="50" t="s">
+      <c r="G118" s="46" t="s">
         <v>450</v>
       </c>
-      <c r="H118" s="50" t="s">
+      <c r="H118" s="46" t="s">
         <v>451</v>
       </c>
-      <c r="I118" s="50" t="s">
+      <c r="I118" s="46" t="s">
         <v>452</v>
       </c>
-      <c r="J118" s="50" t="s">
+      <c r="J118" s="46" t="s">
         <v>453</v>
       </c>
-      <c r="K118" s="50"/>
-      <c r="L118" s="50"/>
-      <c r="M118" s="51"/>
-    </row>
-    <row r="119" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B119" s="49" t="s">
+      <c r="K118" s="46"/>
+      <c r="L118" s="46"/>
+      <c r="M118" s="47"/>
+    </row>
+    <row r="119" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B119" s="45" t="s">
         <v>118</v>
       </c>
-      <c r="C119" s="50" t="s">
+      <c r="C119" s="46" t="s">
         <v>454</v>
       </c>
-      <c r="D119" s="50" t="s">
+      <c r="D119" s="46" t="s">
         <v>455</v>
       </c>
-      <c r="E119" s="50" t="s">
+      <c r="E119" s="46" t="s">
         <v>456</v>
       </c>
-      <c r="F119" s="50" t="s">
+      <c r="F119" s="46" t="s">
         <v>457</v>
       </c>
-      <c r="G119" s="50" t="s">
+      <c r="G119" s="46" t="s">
         <v>458</v>
       </c>
-      <c r="H119" s="50" t="s">
+      <c r="H119" s="46" t="s">
         <v>459</v>
       </c>
-      <c r="I119" s="50" t="s">
+      <c r="I119" s="46" t="s">
         <v>460</v>
       </c>
-      <c r="J119" s="50" t="s">
+      <c r="J119" s="46" t="s">
         <v>461</v>
       </c>
-      <c r="K119" s="50"/>
-      <c r="L119" s="50"/>
-      <c r="M119" s="51"/>
-    </row>
-    <row r="120" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B120" s="49" t="s">
+      <c r="K119" s="46"/>
+      <c r="L119" s="46"/>
+      <c r="M119" s="47"/>
+    </row>
+    <row r="120" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B120" s="45" t="s">
         <v>111</v>
       </c>
-      <c r="C120" s="50" t="s">
+      <c r="C120" s="46" t="s">
         <v>462</v>
       </c>
-      <c r="D120" s="50" t="s">
+      <c r="D120" s="46" t="s">
         <v>463</v>
       </c>
-      <c r="E120" s="50" t="s">
+      <c r="E120" s="46" t="s">
         <v>464</v>
       </c>
-      <c r="F120" s="50" t="s">
+      <c r="F120" s="46" t="s">
         <v>465</v>
       </c>
-      <c r="G120" s="50" t="s">
+      <c r="G120" s="46" t="s">
         <v>466</v>
       </c>
-      <c r="H120" s="50" t="s">
+      <c r="H120" s="46" t="s">
         <v>467</v>
       </c>
-      <c r="I120" s="50" t="s">
+      <c r="I120" s="46" t="s">
         <v>468</v>
       </c>
-      <c r="J120" s="50" t="s">
+      <c r="J120" s="46" t="s">
         <v>469</v>
       </c>
-      <c r="K120" s="50"/>
-      <c r="L120" s="50"/>
-      <c r="M120" s="51"/>
-    </row>
-    <row r="121" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B121" s="49" t="s">
+      <c r="K120" s="46"/>
+      <c r="L120" s="46"/>
+      <c r="M120" s="47"/>
+    </row>
+    <row r="121" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B121" s="45" t="s">
         <v>127</v>
       </c>
-      <c r="C121" s="50" t="s">
+      <c r="C121" s="46" t="s">
         <v>470</v>
       </c>
-      <c r="D121" s="50" t="s">
+      <c r="D121" s="46" t="s">
         <v>471</v>
       </c>
-      <c r="E121" s="50" t="s">
+      <c r="E121" s="46" t="s">
         <v>472</v>
       </c>
-      <c r="F121" s="50" t="s">
+      <c r="F121" s="46" t="s">
         <v>473</v>
       </c>
-      <c r="G121" s="50" t="s">
+      <c r="G121" s="46" t="s">
         <v>474</v>
       </c>
-      <c r="H121" s="50" t="s">
+      <c r="H121" s="46" t="s">
         <v>475</v>
       </c>
-      <c r="I121" s="50" t="s">
+      <c r="I121" s="46" t="s">
         <v>476</v>
       </c>
-      <c r="J121" s="50" t="s">
+      <c r="J121" s="46" t="s">
         <v>477</v>
       </c>
-      <c r="K121" s="50"/>
-      <c r="L121" s="50"/>
-      <c r="M121" s="51"/>
-    </row>
-    <row r="122" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B122" s="49" t="s">
+      <c r="K121" s="46"/>
+      <c r="L121" s="46"/>
+      <c r="M121" s="47"/>
+    </row>
+    <row r="122" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B122" s="45" t="s">
         <v>137</v>
       </c>
-      <c r="C122" s="50" t="s">
+      <c r="C122" s="46" t="s">
         <v>478</v>
       </c>
-      <c r="D122" s="50" t="s">
+      <c r="D122" s="46" t="s">
         <v>479</v>
       </c>
-      <c r="E122" s="50" t="s">
+      <c r="E122" s="46" t="s">
         <v>480</v>
       </c>
-      <c r="F122" s="50" t="s">
+      <c r="F122" s="46" t="s">
         <v>481</v>
       </c>
-      <c r="G122" s="50" t="s">
+      <c r="G122" s="46" t="s">
         <v>482</v>
       </c>
-      <c r="H122" s="50" t="s">
+      <c r="H122" s="46" t="s">
         <v>483</v>
       </c>
-      <c r="I122" s="50" t="s">
+      <c r="I122" s="46" t="s">
         <v>484</v>
       </c>
-      <c r="J122" s="50" t="s">
+      <c r="J122" s="46" t="s">
         <v>485</v>
       </c>
-      <c r="K122" s="50"/>
-      <c r="L122" s="50"/>
-      <c r="M122" s="51"/>
-    </row>
-    <row r="123" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B123" s="49" t="s">
+      <c r="K122" s="46"/>
+      <c r="L122" s="46"/>
+      <c r="M122" s="47"/>
+    </row>
+    <row r="123" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B123" s="45" t="s">
         <v>162</v>
       </c>
-      <c r="C123" s="50" t="s">
+      <c r="C123" s="46" t="s">
         <v>486</v>
       </c>
-      <c r="D123" s="50" t="s">
+      <c r="D123" s="46" t="s">
         <v>487</v>
       </c>
-      <c r="E123" s="50" t="s">
+      <c r="E123" s="46" t="s">
         <v>488</v>
       </c>
-      <c r="F123" s="50" t="s">
+      <c r="F123" s="46" t="s">
         <v>489</v>
       </c>
-      <c r="G123" s="50" t="s">
+      <c r="G123" s="46" t="s">
         <v>490</v>
       </c>
-      <c r="H123" s="50" t="s">
+      <c r="H123" s="46" t="s">
         <v>491</v>
       </c>
-      <c r="I123" s="50" t="s">
+      <c r="I123" s="46" t="s">
         <v>492</v>
       </c>
-      <c r="J123" s="50" t="s">
+      <c r="J123" s="46" t="s">
         <v>493</v>
       </c>
-      <c r="K123" s="50"/>
-      <c r="L123" s="50"/>
-      <c r="M123" s="51"/>
-    </row>
-    <row r="124" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B124" s="49" t="s">
+      <c r="K123" s="46"/>
+      <c r="L123" s="46"/>
+      <c r="M123" s="47"/>
+    </row>
+    <row r="124" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B124" s="45" t="s">
         <v>157</v>
       </c>
-      <c r="C124" s="50" t="s">
+      <c r="C124" s="46" t="s">
         <v>494</v>
       </c>
-      <c r="D124" s="50" t="s">
+      <c r="D124" s="46" t="s">
         <v>495</v>
       </c>
-      <c r="E124" s="50" t="s">
+      <c r="E124" s="46" t="s">
         <v>496</v>
       </c>
-      <c r="F124" s="50" t="s">
+      <c r="F124" s="46" t="s">
         <v>497</v>
       </c>
-      <c r="G124" s="50" t="s">
+      <c r="G124" s="46" t="s">
         <v>498</v>
       </c>
-      <c r="H124" s="50" t="s">
+      <c r="H124" s="46" t="s">
         <v>499</v>
       </c>
-      <c r="I124" s="50" t="s">
+      <c r="I124" s="46" t="s">
         <v>500</v>
       </c>
-      <c r="J124" s="50" t="s">
+      <c r="J124" s="46" t="s">
         <v>501</v>
       </c>
-      <c r="K124" s="50"/>
-      <c r="L124" s="50"/>
-      <c r="M124" s="51"/>
-    </row>
-    <row r="125" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B125" s="49" t="s">
+      <c r="K124" s="46"/>
+      <c r="L124" s="46"/>
+      <c r="M124" s="47"/>
+    </row>
+    <row r="125" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B125" s="45" t="s">
         <v>139</v>
       </c>
-      <c r="C125" s="50" t="s">
+      <c r="C125" s="46" t="s">
         <v>502</v>
       </c>
-      <c r="D125" s="50" t="s">
+      <c r="D125" s="46" t="s">
         <v>503</v>
       </c>
-      <c r="E125" s="50" t="s">
+      <c r="E125" s="46" t="s">
         <v>504</v>
       </c>
-      <c r="F125" s="50" t="s">
+      <c r="F125" s="46" t="s">
         <v>505</v>
       </c>
-      <c r="G125" s="50" t="s">
+      <c r="G125" s="46" t="s">
         <v>506</v>
       </c>
-      <c r="H125" s="50" t="s">
+      <c r="H125" s="46" t="s">
         <v>507</v>
       </c>
-      <c r="I125" s="50" t="s">
+      <c r="I125" s="46" t="s">
         <v>508</v>
       </c>
-      <c r="J125" s="50" t="s">
+      <c r="J125" s="46" t="s">
         <v>509</v>
       </c>
-      <c r="K125" s="50"/>
-      <c r="L125" s="50"/>
-      <c r="M125" s="51"/>
-    </row>
-    <row r="126" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B126" s="49" t="s">
+      <c r="K125" s="46"/>
+      <c r="L125" s="46"/>
+      <c r="M125" s="47"/>
+    </row>
+    <row r="126" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B126" s="45" t="s">
         <v>125</v>
       </c>
-      <c r="C126" s="50" t="s">
+      <c r="C126" s="46" t="s">
         <v>510</v>
       </c>
-      <c r="D126" s="50" t="s">
+      <c r="D126" s="46" t="s">
         <v>511</v>
       </c>
-      <c r="E126" s="50" t="s">
+      <c r="E126" s="46" t="s">
         <v>512</v>
       </c>
-      <c r="F126" s="50" t="s">
+      <c r="F126" s="46" t="s">
         <v>513</v>
       </c>
-      <c r="G126" s="50" t="s">
+      <c r="G126" s="46" t="s">
         <v>514</v>
       </c>
-      <c r="H126" s="50" t="s">
+      <c r="H126" s="46" t="s">
         <v>515</v>
       </c>
-      <c r="I126" s="50" t="s">
+      <c r="I126" s="46" t="s">
         <v>516</v>
       </c>
-      <c r="J126" s="50" t="s">
+      <c r="J126" s="46" t="s">
         <v>517</v>
       </c>
-      <c r="K126" s="50"/>
-      <c r="L126" s="50"/>
-      <c r="M126" s="51"/>
-    </row>
-    <row r="127" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B127" s="49" t="s">
+      <c r="K126" s="46"/>
+      <c r="L126" s="46"/>
+      <c r="M126" s="47"/>
+    </row>
+    <row r="127" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B127" s="45" t="s">
         <v>144</v>
       </c>
-      <c r="C127" s="50" t="s">
+      <c r="C127" s="46" t="s">
         <v>518</v>
       </c>
-      <c r="D127" s="50" t="s">
+      <c r="D127" s="46" t="s">
         <v>519</v>
       </c>
-      <c r="E127" s="50" t="s">
+      <c r="E127" s="46" t="s">
         <v>520</v>
       </c>
-      <c r="F127" s="50" t="s">
+      <c r="F127" s="46" t="s">
         <v>521</v>
       </c>
-      <c r="G127" s="50" t="s">
+      <c r="G127" s="46" t="s">
         <v>522</v>
       </c>
-      <c r="H127" s="50" t="s">
+      <c r="H127" s="46" t="s">
         <v>523</v>
       </c>
-      <c r="I127" s="50" t="s">
+      <c r="I127" s="46" t="s">
         <v>524</v>
       </c>
-      <c r="J127" s="50" t="s">
+      <c r="J127" s="46" t="s">
         <v>525</v>
       </c>
-      <c r="K127" s="50"/>
-      <c r="L127" s="50"/>
-      <c r="M127" s="51"/>
-    </row>
-    <row r="128" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B128" s="49" t="s">
+      <c r="K127" s="46"/>
+      <c r="L127" s="46"/>
+      <c r="M127" s="47"/>
+    </row>
+    <row r="128" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B128" s="45" t="s">
         <v>123</v>
       </c>
-      <c r="C128" s="50" t="s">
+      <c r="C128" s="46" t="s">
         <v>526</v>
       </c>
-      <c r="D128" s="50" t="s">
+      <c r="D128" s="46" t="s">
         <v>527</v>
       </c>
-      <c r="E128" s="50" t="s">
+      <c r="E128" s="46" t="s">
         <v>528</v>
       </c>
-      <c r="F128" s="50" t="s">
+      <c r="F128" s="46" t="s">
         <v>529</v>
       </c>
-      <c r="G128" s="50" t="s">
+      <c r="G128" s="46" t="s">
         <v>530</v>
       </c>
-      <c r="H128" s="50" t="s">
+      <c r="H128" s="46" t="s">
         <v>531</v>
       </c>
-      <c r="I128" s="50" t="s">
+      <c r="I128" s="46" t="s">
         <v>532</v>
       </c>
-      <c r="J128" s="50" t="s">
+      <c r="J128" s="46" t="s">
         <v>533</v>
       </c>
-      <c r="K128" s="50"/>
-      <c r="L128" s="50"/>
-      <c r="M128" s="51"/>
-    </row>
-    <row r="129" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B129" s="49" t="s">
+      <c r="K128" s="46"/>
+      <c r="L128" s="46"/>
+      <c r="M128" s="47"/>
+    </row>
+    <row r="129" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B129" s="45" t="s">
         <v>166</v>
       </c>
-      <c r="C129" s="50" t="s">
+      <c r="C129" s="46" t="s">
         <v>534</v>
       </c>
-      <c r="D129" s="50" t="s">
+      <c r="D129" s="46" t="s">
         <v>535</v>
       </c>
-      <c r="E129" s="50" t="s">
+      <c r="E129" s="46" t="s">
         <v>536</v>
       </c>
-      <c r="F129" s="50" t="s">
+      <c r="F129" s="46" t="s">
         <v>537</v>
       </c>
-      <c r="G129" s="50" t="s">
+      <c r="G129" s="46" t="s">
         <v>538</v>
       </c>
-      <c r="H129" s="50" t="s">
+      <c r="H129" s="46" t="s">
         <v>539</v>
       </c>
-      <c r="I129" s="50" t="s">
+      <c r="I129" s="46" t="s">
         <v>540</v>
       </c>
-      <c r="J129" s="50" t="s">
+      <c r="J129" s="46" t="s">
         <v>541</v>
       </c>
-      <c r="K129" s="50"/>
-      <c r="L129" s="50"/>
-      <c r="M129" s="51"/>
-    </row>
-    <row r="130" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B130" s="49" t="s">
+      <c r="K129" s="46"/>
+      <c r="L129" s="46"/>
+      <c r="M129" s="47"/>
+    </row>
+    <row r="130" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B130" s="45" t="s">
         <v>163</v>
       </c>
-      <c r="C130" s="50" t="s">
+      <c r="C130" s="46" t="s">
         <v>542</v>
       </c>
-      <c r="D130" s="50" t="s">
+      <c r="D130" s="46" t="s">
         <v>543</v>
       </c>
-      <c r="E130" s="50" t="s">
+      <c r="E130" s="46" t="s">
         <v>544</v>
       </c>
-      <c r="F130" s="50" t="s">
+      <c r="F130" s="46" t="s">
         <v>545</v>
       </c>
-      <c r="G130" s="50" t="s">
+      <c r="G130" s="46" t="s">
         <v>546</v>
       </c>
-      <c r="H130" s="50" t="s">
+      <c r="H130" s="46" t="s">
         <v>547</v>
       </c>
-      <c r="I130" s="50" t="s">
+      <c r="I130" s="46" t="s">
         <v>548</v>
       </c>
-      <c r="J130" s="50" t="s">
+      <c r="J130" s="46" t="s">
         <v>549</v>
       </c>
-      <c r="K130" s="50"/>
-      <c r="L130" s="50"/>
-      <c r="M130" s="51"/>
-    </row>
-    <row r="131" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B131" s="49" t="s">
+      <c r="K130" s="46"/>
+      <c r="L130" s="46"/>
+      <c r="M130" s="47"/>
+    </row>
+    <row r="131" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B131" s="45" t="s">
         <v>115</v>
       </c>
-      <c r="C131" s="50" t="s">
+      <c r="C131" s="46" t="s">
         <v>550</v>
       </c>
-      <c r="D131" s="50" t="s">
+      <c r="D131" s="46" t="s">
         <v>551</v>
       </c>
-      <c r="E131" s="50" t="s">
+      <c r="E131" s="46" t="s">
         <v>552</v>
       </c>
-      <c r="F131" s="50" t="s">
+      <c r="F131" s="46" t="s">
         <v>553</v>
       </c>
-      <c r="G131" s="50" t="s">
+      <c r="G131" s="46" t="s">
         <v>554</v>
       </c>
-      <c r="H131" s="50" t="s">
+      <c r="H131" s="46" t="s">
         <v>555</v>
       </c>
-      <c r="I131" s="50" t="s">
+      <c r="I131" s="46" t="s">
         <v>556</v>
       </c>
-      <c r="J131" s="50" t="s">
+      <c r="J131" s="46" t="s">
         <v>557</v>
       </c>
-      <c r="K131" s="50"/>
-      <c r="L131" s="50"/>
-      <c r="M131" s="51"/>
-    </row>
-    <row r="132" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B132" s="49" t="s">
+      <c r="K131" s="46"/>
+      <c r="L131" s="46"/>
+      <c r="M131" s="47"/>
+    </row>
+    <row r="132" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B132" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="C132" s="50" t="s">
+      <c r="C132" s="46" t="s">
         <v>558</v>
       </c>
-      <c r="D132" s="50" t="s">
+      <c r="D132" s="46" t="s">
         <v>559</v>
       </c>
-      <c r="E132" s="50" t="s">
+      <c r="E132" s="46" t="s">
         <v>560</v>
       </c>
-      <c r="F132" s="50" t="s">
+      <c r="F132" s="46" t="s">
         <v>561</v>
       </c>
-      <c r="G132" s="50" t="s">
+      <c r="G132" s="46" t="s">
         <v>562</v>
       </c>
-      <c r="H132" s="50" t="s">
+      <c r="H132" s="46" t="s">
         <v>563</v>
       </c>
-      <c r="I132" s="50" t="s">
+      <c r="I132" s="46" t="s">
         <v>564</v>
       </c>
-      <c r="J132" s="50" t="s">
+      <c r="J132" s="46" t="s">
         <v>565</v>
       </c>
-      <c r="K132" s="50"/>
-      <c r="L132" s="50"/>
-      <c r="M132" s="51"/>
-    </row>
-    <row r="133" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B133" s="49" t="s">
+      <c r="K132" s="46"/>
+      <c r="L132" s="46"/>
+      <c r="M132" s="47"/>
+    </row>
+    <row r="133" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B133" s="45" t="s">
         <v>153</v>
       </c>
-      <c r="C133" s="50" t="s">
+      <c r="C133" s="46" t="s">
         <v>566</v>
       </c>
-      <c r="D133" s="50" t="s">
+      <c r="D133" s="46" t="s">
         <v>567</v>
       </c>
-      <c r="E133" s="50" t="s">
+      <c r="E133" s="46" t="s">
         <v>568</v>
       </c>
-      <c r="F133" s="50" t="s">
+      <c r="F133" s="46" t="s">
         <v>569</v>
       </c>
-      <c r="G133" s="50" t="s">
+      <c r="G133" s="46" t="s">
         <v>570</v>
       </c>
-      <c r="H133" s="50" t="s">
+      <c r="H133" s="46" t="s">
         <v>571</v>
       </c>
-      <c r="I133" s="50" t="s">
+      <c r="I133" s="46" t="s">
         <v>572</v>
       </c>
-      <c r="J133" s="50" t="s">
+      <c r="J133" s="46" t="s">
         <v>573</v>
       </c>
-      <c r="K133" s="50"/>
-      <c r="L133" s="50"/>
-      <c r="M133" s="51"/>
-    </row>
-    <row r="134" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B134" s="49" t="s">
+      <c r="K133" s="46"/>
+      <c r="L133" s="46"/>
+      <c r="M133" s="47"/>
+    </row>
+    <row r="134" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B134" s="45" t="s">
         <v>136</v>
       </c>
-      <c r="C134" s="50" t="s">
+      <c r="C134" s="46" t="s">
         <v>574</v>
       </c>
-      <c r="D134" s="50" t="s">
+      <c r="D134" s="46" t="s">
         <v>575</v>
       </c>
-      <c r="E134" s="50" t="s">
+      <c r="E134" s="46" t="s">
         <v>576</v>
       </c>
-      <c r="F134" s="50" t="s">
+      <c r="F134" s="46" t="s">
         <v>577</v>
       </c>
-      <c r="G134" s="50" t="s">
+      <c r="G134" s="46" t="s">
         <v>578</v>
       </c>
-      <c r="H134" s="50" t="s">
+      <c r="H134" s="46" t="s">
         <v>579</v>
       </c>
-      <c r="I134" s="50" t="s">
+      <c r="I134" s="46" t="s">
         <v>580</v>
       </c>
-      <c r="J134" s="50" t="s">
+      <c r="J134" s="46" t="s">
         <v>581</v>
       </c>
-      <c r="K134" s="50"/>
-      <c r="L134" s="50"/>
-      <c r="M134" s="51"/>
-    </row>
-    <row r="135" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B135" s="49" t="s">
+      <c r="K134" s="46"/>
+      <c r="L134" s="46"/>
+      <c r="M134" s="47"/>
+    </row>
+    <row r="135" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B135" s="45" t="s">
         <v>141</v>
       </c>
-      <c r="C135" s="50" t="s">
+      <c r="C135" s="46" t="s">
         <v>582</v>
       </c>
-      <c r="D135" s="50" t="s">
+      <c r="D135" s="46" t="s">
         <v>583</v>
       </c>
-      <c r="E135" s="50" t="s">
+      <c r="E135" s="46" t="s">
         <v>584</v>
       </c>
-      <c r="F135" s="50" t="s">
+      <c r="F135" s="46" t="s">
         <v>585</v>
       </c>
-      <c r="G135" s="50" t="s">
+      <c r="G135" s="46" t="s">
         <v>586</v>
       </c>
-      <c r="H135" s="50" t="s">
+      <c r="H135" s="46" t="s">
         <v>587</v>
       </c>
-      <c r="I135" s="50" t="s">
+      <c r="I135" s="46" t="s">
         <v>588</v>
       </c>
-      <c r="J135" s="50" t="s">
+      <c r="J135" s="46" t="s">
         <v>589</v>
       </c>
-      <c r="K135" s="50"/>
-      <c r="L135" s="50"/>
-      <c r="M135" s="51"/>
-    </row>
-    <row r="136" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B136" s="49" t="s">
+      <c r="K135" s="46"/>
+      <c r="L135" s="46"/>
+      <c r="M135" s="47"/>
+    </row>
+    <row r="136" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B136" s="45" t="s">
         <v>150</v>
       </c>
-      <c r="C136" s="50" t="s">
+      <c r="C136" s="46" t="s">
         <v>590</v>
       </c>
-      <c r="D136" s="50" t="s">
+      <c r="D136" s="46" t="s">
         <v>591</v>
       </c>
-      <c r="E136" s="50" t="s">
+      <c r="E136" s="46" t="s">
         <v>592</v>
       </c>
-      <c r="F136" s="50" t="s">
+      <c r="F136" s="46" t="s">
         <v>593</v>
       </c>
-      <c r="G136" s="50" t="s">
+      <c r="G136" s="46" t="s">
         <v>594</v>
       </c>
-      <c r="H136" s="50" t="s">
+      <c r="H136" s="46" t="s">
         <v>595</v>
       </c>
-      <c r="I136" s="50" t="s">
+      <c r="I136" s="46" t="s">
         <v>596</v>
       </c>
-      <c r="J136" s="50" t="s">
+      <c r="J136" s="46" t="s">
         <v>597</v>
       </c>
-      <c r="K136" s="50"/>
-      <c r="L136" s="50"/>
-      <c r="M136" s="51"/>
-    </row>
-    <row r="137" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B137" s="49" t="s">
+      <c r="K136" s="46"/>
+      <c r="L136" s="46"/>
+      <c r="M136" s="47"/>
+    </row>
+    <row r="137" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B137" s="45" t="s">
         <v>598</v>
       </c>
-      <c r="C137" s="50" t="s">
+      <c r="C137" s="46" t="s">
         <v>599</v>
       </c>
-      <c r="D137" s="50" t="s">
+      <c r="D137" s="46" t="s">
         <v>455</v>
       </c>
-      <c r="E137" s="50" t="s">
+      <c r="E137" s="46" t="s">
         <v>600</v>
       </c>
-      <c r="F137" s="50" t="s">
+      <c r="F137" s="46" t="s">
         <v>601</v>
       </c>
-      <c r="G137" s="50" t="s">
+      <c r="G137" s="46" t="s">
         <v>602</v>
       </c>
-      <c r="H137" s="50" t="s">
+      <c r="H137" s="46" t="s">
         <v>603</v>
       </c>
-      <c r="I137" s="50" t="s">
+      <c r="I137" s="46" t="s">
         <v>604</v>
       </c>
-      <c r="J137" s="50" t="s">
+      <c r="J137" s="46" t="s">
         <v>605</v>
       </c>
-      <c r="K137" s="50"/>
-      <c r="L137" s="50"/>
-      <c r="M137" s="51"/>
-    </row>
-    <row r="138" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B138" s="49" t="s">
+      <c r="K137" s="46"/>
+      <c r="L137" s="46"/>
+      <c r="M137" s="47"/>
+    </row>
+    <row r="138" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B138" s="45" t="s">
         <v>117</v>
       </c>
-      <c r="C138" s="50" t="s">
+      <c r="C138" s="46" t="s">
         <v>606</v>
       </c>
-      <c r="D138" s="50" t="s">
+      <c r="D138" s="46" t="s">
         <v>607</v>
       </c>
-      <c r="E138" s="50" t="s">
+      <c r="E138" s="46" t="s">
         <v>608</v>
       </c>
-      <c r="F138" s="50" t="s">
+      <c r="F138" s="46" t="s">
         <v>609</v>
       </c>
-      <c r="G138" s="50" t="s">
+      <c r="G138" s="46" t="s">
         <v>610</v>
       </c>
-      <c r="H138" s="50" t="s">
+      <c r="H138" s="46" t="s">
         <v>611</v>
       </c>
-      <c r="I138" s="50" t="s">
+      <c r="I138" s="46" t="s">
         <v>612</v>
       </c>
-      <c r="J138" s="50" t="s">
+      <c r="J138" s="46" t="s">
         <v>613</v>
       </c>
-      <c r="K138" s="50"/>
-      <c r="L138" s="50"/>
-      <c r="M138" s="51"/>
-    </row>
-    <row r="139" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B139" s="49" t="s">
+      <c r="K138" s="46"/>
+      <c r="L138" s="46"/>
+      <c r="M138" s="47"/>
+    </row>
+    <row r="139" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B139" s="45" t="s">
         <v>614</v>
       </c>
-      <c r="C139" s="50" t="s">
+      <c r="C139" s="46" t="s">
         <v>615</v>
       </c>
-      <c r="D139" s="50" t="s">
+      <c r="D139" s="46" t="s">
         <v>616</v>
       </c>
-      <c r="E139" s="50" t="s">
+      <c r="E139" s="46" t="s">
         <v>617</v>
       </c>
-      <c r="F139" s="50" t="s">
+      <c r="F139" s="46" t="s">
         <v>618</v>
       </c>
-      <c r="G139" s="50" t="s">
+      <c r="G139" s="46" t="s">
         <v>619</v>
       </c>
-      <c r="H139" s="50" t="s">
+      <c r="H139" s="46" t="s">
         <v>620</v>
       </c>
-      <c r="I139" s="50" t="s">
+      <c r="I139" s="46" t="s">
         <v>621</v>
       </c>
-      <c r="J139" s="50" t="s">
+      <c r="J139" s="46" t="s">
         <v>622</v>
       </c>
-      <c r="K139" s="50"/>
-      <c r="L139" s="50"/>
-      <c r="M139" s="51"/>
-    </row>
-    <row r="140" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B140" s="49" t="s">
+      <c r="K139" s="46"/>
+      <c r="L139" s="46"/>
+      <c r="M139" s="47"/>
+    </row>
+    <row r="140" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B140" s="45" t="s">
         <v>132</v>
       </c>
-      <c r="C140" s="50" t="s">
+      <c r="C140" s="46" t="s">
         <v>623</v>
       </c>
-      <c r="D140" s="50" t="s">
+      <c r="D140" s="46" t="s">
         <v>624</v>
       </c>
-      <c r="E140" s="50" t="s">
+      <c r="E140" s="46" t="s">
         <v>625</v>
       </c>
-      <c r="F140" s="50" t="s">
+      <c r="F140" s="46" t="s">
         <v>626</v>
       </c>
-      <c r="G140" s="50" t="s">
+      <c r="G140" s="46" t="s">
         <v>627</v>
       </c>
-      <c r="H140" s="50" t="s">
+      <c r="H140" s="46" t="s">
         <v>628</v>
       </c>
-      <c r="I140" s="50" t="s">
+      <c r="I140" s="46" t="s">
         <v>629</v>
       </c>
-      <c r="J140" s="50" t="s">
+      <c r="J140" s="46" t="s">
         <v>630</v>
       </c>
-      <c r="K140" s="50"/>
-      <c r="L140" s="50"/>
-      <c r="M140" s="51"/>
-    </row>
-    <row r="141" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B141" s="49" t="s">
+      <c r="K140" s="46"/>
+      <c r="L140" s="46"/>
+      <c r="M140" s="47"/>
+    </row>
+    <row r="141" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B141" s="45" t="s">
         <v>631</v>
       </c>
-      <c r="C141" s="50" t="s">
+      <c r="C141" s="46" t="s">
         <v>632</v>
       </c>
-      <c r="D141" s="50" t="s">
+      <c r="D141" s="46" t="s">
         <v>633</v>
       </c>
-      <c r="E141" s="50" t="s">
+      <c r="E141" s="46" t="s">
         <v>634</v>
       </c>
-      <c r="F141" s="50" t="s">
+      <c r="F141" s="46" t="s">
         <v>635</v>
       </c>
-      <c r="G141" s="50" t="s">
+      <c r="G141" s="46" t="s">
         <v>636</v>
       </c>
-      <c r="H141" s="50" t="s">
+      <c r="H141" s="46" t="s">
         <v>637</v>
       </c>
-      <c r="I141" s="50" t="s">
+      <c r="I141" s="46" t="s">
         <v>638</v>
       </c>
-      <c r="J141" s="50" t="s">
+      <c r="J141" s="46" t="s">
         <v>639</v>
       </c>
-      <c r="K141" s="50"/>
-      <c r="L141" s="50"/>
-      <c r="M141" s="51"/>
-    </row>
-    <row r="142" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B142" s="49" t="s">
+      <c r="K141" s="46"/>
+      <c r="L141" s="46"/>
+      <c r="M141" s="47"/>
+    </row>
+    <row r="142" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B142" s="45" t="s">
         <v>168</v>
       </c>
-      <c r="C142" s="50" t="s">
+      <c r="C142" s="46" t="s">
         <v>640</v>
       </c>
-      <c r="D142" s="50" t="s">
+      <c r="D142" s="46" t="s">
         <v>641</v>
       </c>
-      <c r="E142" s="50" t="s">
+      <c r="E142" s="46" t="s">
         <v>642</v>
       </c>
-      <c r="F142" s="50" t="s">
+      <c r="F142" s="46" t="s">
         <v>643</v>
       </c>
-      <c r="G142" s="50" t="s">
+      <c r="G142" s="46" t="s">
         <v>644</v>
       </c>
-      <c r="H142" s="50" t="s">
+      <c r="H142" s="46" t="s">
         <v>645</v>
       </c>
-      <c r="I142" s="50" t="s">
+      <c r="I142" s="46" t="s">
         <v>646</v>
       </c>
-      <c r="J142" s="50" t="s">
+      <c r="J142" s="46" t="s">
         <v>647</v>
       </c>
-      <c r="K142" s="50"/>
-      <c r="L142" s="50"/>
-      <c r="M142" s="51"/>
-    </row>
-    <row r="143" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B143" s="49" t="s">
+      <c r="K142" s="46"/>
+      <c r="L142" s="46"/>
+      <c r="M142" s="47"/>
+    </row>
+    <row r="143" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B143" s="45" t="s">
         <v>156</v>
       </c>
-      <c r="C143" s="50" t="s">
+      <c r="C143" s="46" t="s">
         <v>648</v>
       </c>
-      <c r="D143" s="50" t="s">
+      <c r="D143" s="46" t="s">
         <v>649</v>
       </c>
-      <c r="E143" s="50" t="s">
+      <c r="E143" s="46" t="s">
         <v>650</v>
       </c>
-      <c r="F143" s="50" t="s">
+      <c r="F143" s="46" t="s">
         <v>651</v>
       </c>
-      <c r="G143" s="50" t="s">
+      <c r="G143" s="46" t="s">
         <v>652</v>
       </c>
-      <c r="H143" s="50" t="s">
+      <c r="H143" s="46" t="s">
         <v>653</v>
       </c>
-      <c r="I143" s="50" t="s">
+      <c r="I143" s="46" t="s">
         <v>654</v>
       </c>
-      <c r="J143" s="50" t="s">
+      <c r="J143" s="46" t="s">
         <v>655</v>
       </c>
-      <c r="K143" s="50"/>
-      <c r="L143" s="50"/>
-      <c r="M143" s="51"/>
-    </row>
-    <row r="144" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B144" s="49" t="s">
+      <c r="K143" s="46"/>
+      <c r="L143" s="46"/>
+      <c r="M143" s="47"/>
+    </row>
+    <row r="144" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B144" s="45" t="s">
         <v>131</v>
       </c>
-      <c r="C144" s="50" t="s">
+      <c r="C144" s="46" t="s">
         <v>656</v>
       </c>
-      <c r="D144" s="50" t="s">
+      <c r="D144" s="46" t="s">
         <v>657</v>
       </c>
-      <c r="E144" s="50" t="s">
+      <c r="E144" s="46" t="s">
         <v>658</v>
       </c>
-      <c r="F144" s="50" t="s">
+      <c r="F144" s="46" t="s">
         <v>659</v>
       </c>
-      <c r="G144" s="50" t="s">
+      <c r="G144" s="46" t="s">
         <v>660</v>
       </c>
-      <c r="H144" s="50" t="s">
+      <c r="H144" s="46" t="s">
         <v>661</v>
       </c>
-      <c r="I144" s="50" t="s">
+      <c r="I144" s="46" t="s">
         <v>662</v>
       </c>
-      <c r="J144" s="50" t="s">
+      <c r="J144" s="46" t="s">
         <v>663</v>
       </c>
-      <c r="K144" s="50"/>
-      <c r="L144" s="50"/>
-      <c r="M144" s="51"/>
-    </row>
-    <row r="145" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B145" s="49" t="s">
+      <c r="K144" s="46"/>
+      <c r="L144" s="46"/>
+      <c r="M144" s="47"/>
+    </row>
+    <row r="145" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B145" s="45" t="s">
         <v>664</v>
       </c>
-      <c r="C145" s="50" t="s">
+      <c r="C145" s="46" t="s">
         <v>665</v>
       </c>
-      <c r="D145" s="50" t="s">
+      <c r="D145" s="46" t="s">
         <v>666</v>
       </c>
-      <c r="E145" s="50" t="s">
+      <c r="E145" s="46" t="s">
         <v>667</v>
       </c>
-      <c r="F145" s="50" t="s">
+      <c r="F145" s="46" t="s">
         <v>668</v>
       </c>
-      <c r="G145" s="50" t="s">
+      <c r="G145" s="46" t="s">
         <v>669</v>
       </c>
-      <c r="H145" s="50" t="s">
+      <c r="H145" s="46" t="s">
         <v>670</v>
       </c>
-      <c r="I145" s="50" t="s">
+      <c r="I145" s="46" t="s">
         <v>671</v>
       </c>
-      <c r="J145" s="50" t="s">
+      <c r="J145" s="46" t="s">
         <v>672</v>
       </c>
-      <c r="K145" s="50"/>
-      <c r="L145" s="50"/>
-      <c r="M145" s="51"/>
-    </row>
-    <row r="146" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B146" s="49" t="s">
+      <c r="K145" s="46"/>
+      <c r="L145" s="46"/>
+      <c r="M145" s="47"/>
+    </row>
+    <row r="146" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B146" s="45" t="s">
         <v>116</v>
       </c>
-      <c r="C146" s="50" t="s">
+      <c r="C146" s="46" t="s">
         <v>673</v>
       </c>
-      <c r="D146" s="50" t="s">
+      <c r="D146" s="46" t="s">
         <v>674</v>
       </c>
-      <c r="E146" s="50" t="s">
+      <c r="E146" s="46" t="s">
         <v>675</v>
       </c>
-      <c r="F146" s="50" t="s">
+      <c r="F146" s="46" t="s">
         <v>676</v>
       </c>
-      <c r="G146" s="50" t="s">
+      <c r="G146" s="46" t="s">
         <v>677</v>
       </c>
-      <c r="H146" s="50" t="s">
+      <c r="H146" s="46" t="s">
         <v>678</v>
       </c>
-      <c r="I146" s="50" t="s">
+      <c r="I146" s="46" t="s">
         <v>679</v>
       </c>
-      <c r="J146" s="50" t="s">
+      <c r="J146" s="46" t="s">
         <v>680</v>
       </c>
-      <c r="K146" s="50"/>
-      <c r="L146" s="50"/>
-      <c r="M146" s="51"/>
-    </row>
-    <row r="147" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B147" s="49" t="s">
+      <c r="K146" s="46"/>
+      <c r="L146" s="46"/>
+      <c r="M146" s="47"/>
+    </row>
+    <row r="147" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B147" s="45" t="s">
         <v>113</v>
       </c>
-      <c r="C147" s="50" t="s">
+      <c r="C147" s="46" t="s">
         <v>681</v>
       </c>
-      <c r="D147" s="50" t="s">
+      <c r="D147" s="46" t="s">
         <v>682</v>
       </c>
-      <c r="E147" s="50" t="s">
+      <c r="E147" s="46" t="s">
         <v>683</v>
       </c>
-      <c r="F147" s="50" t="s">
+      <c r="F147" s="46" t="s">
         <v>684</v>
       </c>
-      <c r="G147" s="50" t="s">
+      <c r="G147" s="46" t="s">
         <v>685</v>
       </c>
-      <c r="H147" s="50" t="s">
+      <c r="H147" s="46" t="s">
         <v>686</v>
       </c>
-      <c r="I147" s="50" t="s">
+      <c r="I147" s="46" t="s">
         <v>687</v>
       </c>
-      <c r="J147" s="50" t="s">
+      <c r="J147" s="46" t="s">
         <v>688</v>
       </c>
-      <c r="K147" s="50"/>
-      <c r="L147" s="50"/>
-      <c r="M147" s="51"/>
-    </row>
-    <row r="148" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B148" s="49" t="s">
+      <c r="K147" s="46"/>
+      <c r="L147" s="46"/>
+      <c r="M147" s="47"/>
+    </row>
+    <row r="148" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B148" s="45" t="s">
         <v>154</v>
       </c>
-      <c r="C148" s="50" t="s">
+      <c r="C148" s="46" t="s">
         <v>689</v>
       </c>
-      <c r="D148" s="50" t="s">
+      <c r="D148" s="46" t="s">
         <v>287</v>
       </c>
-      <c r="E148" s="50" t="s">
+      <c r="E148" s="46" t="s">
         <v>690</v>
       </c>
-      <c r="F148" s="50" t="s">
+      <c r="F148" s="46" t="s">
         <v>691</v>
       </c>
-      <c r="G148" s="50" t="s">
+      <c r="G148" s="46" t="s">
         <v>692</v>
       </c>
-      <c r="H148" s="50" t="s">
+      <c r="H148" s="46" t="s">
         <v>693</v>
       </c>
-      <c r="I148" s="50" t="s">
+      <c r="I148" s="46" t="s">
         <v>694</v>
       </c>
-      <c r="J148" s="50" t="s">
+      <c r="J148" s="46" t="s">
         <v>695</v>
       </c>
-      <c r="K148" s="50"/>
-      <c r="L148" s="50"/>
-      <c r="M148" s="51"/>
-    </row>
-    <row r="149" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B149" s="49" t="s">
+      <c r="K148" s="46"/>
+      <c r="L148" s="46"/>
+      <c r="M148" s="47"/>
+    </row>
+    <row r="149" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B149" s="45" t="s">
         <v>145</v>
       </c>
-      <c r="C149" s="50" t="s">
+      <c r="C149" s="46" t="s">
         <v>696</v>
       </c>
-      <c r="D149" s="50" t="s">
+      <c r="D149" s="46" t="s">
         <v>697</v>
       </c>
-      <c r="E149" s="50" t="s">
+      <c r="E149" s="46" t="s">
         <v>698</v>
       </c>
-      <c r="F149" s="50" t="s">
+      <c r="F149" s="46" t="s">
         <v>699</v>
       </c>
-      <c r="G149" s="50" t="s">
+      <c r="G149" s="46" t="s">
         <v>700</v>
       </c>
-      <c r="H149" s="50" t="s">
+      <c r="H149" s="46" t="s">
         <v>701</v>
       </c>
-      <c r="I149" s="50" t="s">
+      <c r="I149" s="46" t="s">
         <v>702</v>
       </c>
-      <c r="J149" s="50" t="s">
+      <c r="J149" s="46" t="s">
         <v>703</v>
       </c>
-      <c r="K149" s="50"/>
-      <c r="L149" s="50"/>
-      <c r="M149" s="51"/>
-    </row>
-    <row r="150" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B150" s="49" t="s">
+      <c r="K149" s="46"/>
+      <c r="L149" s="46"/>
+      <c r="M149" s="47"/>
+    </row>
+    <row r="150" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B150" s="45" t="s">
         <v>158</v>
       </c>
-      <c r="C150" s="50" t="s">
+      <c r="C150" s="46" t="s">
         <v>704</v>
       </c>
-      <c r="D150" s="50" t="s">
+      <c r="D150" s="46" t="s">
         <v>705</v>
       </c>
-      <c r="E150" s="50" t="s">
+      <c r="E150" s="46" t="s">
         <v>706</v>
       </c>
-      <c r="F150" s="50" t="s">
+      <c r="F150" s="46" t="s">
         <v>707</v>
       </c>
-      <c r="G150" s="50" t="s">
+      <c r="G150" s="46" t="s">
         <v>708</v>
       </c>
-      <c r="H150" s="50" t="s">
+      <c r="H150" s="46" t="s">
         <v>709</v>
       </c>
-      <c r="I150" s="50" t="s">
+      <c r="I150" s="46" t="s">
         <v>710</v>
       </c>
-      <c r="J150" s="50" t="s">
+      <c r="J150" s="46" t="s">
         <v>711</v>
       </c>
-      <c r="K150" s="50"/>
-      <c r="L150" s="50"/>
-      <c r="M150" s="51"/>
-    </row>
-    <row r="151" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B151" s="49" t="s">
+      <c r="K150" s="46"/>
+      <c r="L150" s="46"/>
+      <c r="M150" s="47"/>
+    </row>
+    <row r="151" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B151" s="45" t="s">
         <v>114</v>
       </c>
-      <c r="C151" s="50" t="s">
+      <c r="C151" s="46" t="s">
         <v>712</v>
       </c>
-      <c r="D151" s="50" t="s">
+      <c r="D151" s="46" t="s">
         <v>713</v>
       </c>
-      <c r="E151" s="50" t="s">
+      <c r="E151" s="46" t="s">
         <v>714</v>
       </c>
-      <c r="F151" s="50" t="s">
+      <c r="F151" s="46" t="s">
         <v>715</v>
       </c>
-      <c r="G151" s="50" t="s">
+      <c r="G151" s="46" t="s">
         <v>716</v>
       </c>
-      <c r="H151" s="50" t="s">
+      <c r="H151" s="46" t="s">
         <v>717</v>
       </c>
-      <c r="I151" s="50" t="s">
+      <c r="I151" s="46" t="s">
         <v>718</v>
       </c>
-      <c r="J151" s="50" t="s">
+      <c r="J151" s="46" t="s">
         <v>719</v>
       </c>
-      <c r="K151" s="50"/>
-      <c r="L151" s="50"/>
-      <c r="M151" s="51"/>
-    </row>
-    <row r="152" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B152" s="49" t="s">
+      <c r="K151" s="46"/>
+      <c r="L151" s="46"/>
+      <c r="M151" s="47"/>
+    </row>
+    <row r="152" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B152" s="45" t="s">
         <v>164</v>
       </c>
-      <c r="C152" s="50" t="s">
+      <c r="C152" s="46" t="s">
         <v>720</v>
       </c>
-      <c r="D152" s="50" t="s">
+      <c r="D152" s="46" t="s">
         <v>721</v>
       </c>
-      <c r="E152" s="50" t="s">
+      <c r="E152" s="46" t="s">
         <v>722</v>
       </c>
-      <c r="F152" s="50" t="s">
+      <c r="F152" s="46" t="s">
         <v>723</v>
       </c>
-      <c r="G152" s="50" t="s">
+      <c r="G152" s="46" t="s">
         <v>724</v>
       </c>
-      <c r="H152" s="50" t="s">
+      <c r="H152" s="46" t="s">
         <v>725</v>
       </c>
-      <c r="I152" s="50" t="s">
+      <c r="I152" s="46" t="s">
         <v>726</v>
       </c>
-      <c r="J152" s="50" t="s">
+      <c r="J152" s="46" t="s">
         <v>727</v>
       </c>
-      <c r="K152" s="50"/>
-      <c r="L152" s="50"/>
-      <c r="M152" s="51"/>
-    </row>
-    <row r="153" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B153" s="49" t="s">
+      <c r="K152" s="46"/>
+      <c r="L152" s="46"/>
+      <c r="M152" s="47"/>
+    </row>
+    <row r="153" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B153" s="45" t="s">
         <v>142</v>
       </c>
-      <c r="C153" s="50" t="s">
+      <c r="C153" s="46" t="s">
         <v>728</v>
       </c>
-      <c r="D153" s="50" t="s">
+      <c r="D153" s="46" t="s">
         <v>729</v>
       </c>
-      <c r="E153" s="50" t="s">
+      <c r="E153" s="46" t="s">
         <v>730</v>
       </c>
-      <c r="F153" s="50" t="s">
+      <c r="F153" s="46" t="s">
         <v>731</v>
       </c>
-      <c r="G153" s="50" t="s">
+      <c r="G153" s="46" t="s">
         <v>732</v>
       </c>
-      <c r="H153" s="50" t="s">
+      <c r="H153" s="46" t="s">
         <v>733</v>
       </c>
-      <c r="I153" s="50" t="s">
+      <c r="I153" s="46" t="s">
         <v>734</v>
       </c>
-      <c r="J153" s="50" t="s">
+      <c r="J153" s="46" t="s">
         <v>735</v>
       </c>
-      <c r="K153" s="50"/>
-      <c r="L153" s="50"/>
-      <c r="M153" s="51"/>
+      <c r="K153" s="46"/>
+      <c r="L153" s="46"/>
+      <c r="M153" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>